<commit_message>
Get daily reddit data: Tue Dec 31 08:10:46 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_05.xlsx
+++ b/data/collected_data/2025_01_05.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C498"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3355 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1hq9jsv</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>My Snake Nails!🐍💖</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq9jsv</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1hq91l3</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you please tell me the pros and cons of Powder Dip over Gel nails? </t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hq91l3/can_you_please_tell_me_the_pros_and_cons_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1hq90k1</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you please tell me the pros and cons of Powder Dip over Gel nails? </t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hq90k1/can_you_please_tell_me_the_pros_and_cons_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1hq8clf</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can someone please tell me the advantages and disadvantage of Dip Nails ? </t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hq8clf/can_someone_please_tell_me_the_advantages_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1hq8v3h</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh color and sparkle </t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq8v3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1hq8rzl</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first French manicure. </t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5qlpaqko4ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1hq8o84</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Manicurist Gel Setting Issue</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hq8o84/manicurist_gel_setting_issue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1hq8g0r</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>What’s a nice high end brand for chrome? I usually use après for polish and like it when my nail products have that sort of level of luxury and high end feeling. Looking for a chrome that can go on solid colors to create a shimmery version of that color and not take it away.</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hq8g0r/whats_a_nice_high_end_brand_for_chrome_i_usually/</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1hq891n</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PLEASE CHOOSE </t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq891n</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1hq7og0</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Nude for every date 🤎</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1z26xemc4ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1hq7mgt</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>OPI Bubble Bath</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hq7mgt/opi_bubble_bath/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1hq79mt</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>✨️ They glowwww! ✨️</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq79mt</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1hq72d0</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>New years nails 🎆</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6ksyatlh64ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1hq5uun</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>just got my nails done, is it supposed to look like this?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq5uun</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1hq665c</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Winter blues</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1hsj1wox3ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1hq65l1</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glitter encapsulation </t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq65l1</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1hq64va</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Roses and chrome</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq64va</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1hq5trh</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>What are the limitations with dip manicures?</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hq5trh/what_are_the_limitations_with_dip_manicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1hq5oje</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>New Set for the New Year</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kpefft61t3ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1hq5e0z</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>NYE nails ✨♥️🍸</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onn5bqm9q3ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1hq5bmz</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What color nails should I do with this dress? </t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pl5t6orhp3ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1hq5773</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>First set in over a year 💜</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ycirs6aco3ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1hq54pz</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>jelly pink. 🩷</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f68z551vn3ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1hq4vrb</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Where can I buy salon supplies without a license?</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hq4vrb/where_can_i_buy_salon_supplies_without_a_license/</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1hq4qge</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Second attempt doing Gel-X at home</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq4qge</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1hq4lu4</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Latest dark tone nailsets</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq4lu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1hq4epr</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Got my nails done!😊</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ti0863z2h3ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1hq4ajh</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Last manicure of the year done by me, what do you think? </t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9wb7n0zf3ae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1hq3wyj</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Glittery gold for new year</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gfhyoznc3ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1hq3tm4</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Help me with my bf’s nails!!</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hq3tm4/help_me_with_my_bfs_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1hq3hk9</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Fallout set</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq3hk9</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1hq3cec</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>What do you think of my new set?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9o4bgx7l73ae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1hq35ea</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Christmas nails 🎄</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t15dve4u53ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1hq3052</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>NYE Nails 🥰💅✨</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq3052</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1hq2xke</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Now I remember why I liked holo taco so much!</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6v64gozx33ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1hq2jy3</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Long coffin black French tips </t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dqtdt5q03ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1hq29jn</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Just feel happy with this crystal ball nail I made for my Christmas nail set</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/indt29t5y2ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1hq26do</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>That 9inches emery board 🔥</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdpgplhgx2ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1hq2264</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>First professional paint job</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq2264</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1hq1san</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>I feel like New Year’s Eve calls for sparkles 🖤✨</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f87fodo7u2ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1hq1l99</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Cost $20 USD in Vietnam</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xed8hgjns2ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1hq1513</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>New years nails, how did I do &lt;3</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq1513</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1hpzvm5</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Starting to notice some real progress with doing my own gels!! Just wish it didn’t take so bloody long </t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8w3eusqxe2ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1hpzypq</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>How do I get my nail polish to look even without trimming my cuticles?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hpzypq/how_do_i_get_my_nail_polish_to_look_even_without/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1hpzw21</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Uneven white part?</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbvwb751f2ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1hpyge2</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Graffiti (handpainted on press-ons)</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpyge2</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1hpyjwh</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>What‘s This Line Going Across My Nail?</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qncef5fl42ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1hpzh0u</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>First time with polygel, I must admit that I really like this material.</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w35b249pb2ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1hpz1q2</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>A nice sleek set for the new year 🤘🏻</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9w6n6pyc82ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1hpyxn7</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>🥂 ILNP Opening Night skittle for NYE (minus Curtain Call, I decided to save that for its own mani). Three coats of each with Spotlight as a topper.</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpyxn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1hpyucy</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>What kinds of nails should I do at home??</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hpyucy/what_kinds_of_nails_should_i_do_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1hpyubw</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>why do I have this random line going across my nail?</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcfq4sar62ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1hpyn4z</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Fresh set for the new year</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/80xsknz852ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1hpy3au</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Sadly one of my nails came off 😫</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzdwrqk112ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1hpy98t</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why did I wait so long?! </t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b21ypqac22ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1hpy39a</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>WWYD?</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hpy39a/wwyd/</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1hpy14d</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving the cat eye </t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ah9mi8vj02ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1hpxwrh</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m a bit obsessed </t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpxwrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1hpxonl</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Brands of 3XL soft gel extensions (square) ???</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hpxonl/brands_of_3xl_soft_gel_extensions_square/</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1hpxj5h</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye </t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpxj5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1hpxeum</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>My artist kills every time 😫</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpxeum</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1hpxei0</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Not your typical post</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xfysczkov1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1hpxddx</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>First time doing my own extensions! Does this length/shape work for me?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gytdmeogv1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1hpxb4o</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>New overlay 🥰</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgdqvqxzu1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1hpx7w1</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Which nail shape suits me better? (Planning on using sapphire polish in last pick for NYE)</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpx7w1</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1hpx5zg</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Love clear polish!</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpx5zg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1hpx3e1</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>The first set I’ve done!</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mei9rfbt1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1hpwo92</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Etsy nails</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8l45r2pzp1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1hpwwzx</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>OPI Wicked promotional colors</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpwwzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1hpwf8f</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New to all of this stuff - can anyone tell me what this is and when to use it? </t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p55hhul2o1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1hpws51</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>First manicure in months! Full gel acrylic set, sparkly periwinkle blue 😊</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpws51</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1hpwrx8</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>NYE Nails🩵</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpwrx8</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1hpwkbk</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>BKIND polish brand reviews?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hpwkbk/bkind_polish_brand_reviews/</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1hpwirs</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Last set of 2024. Decided to end on a sparkly note</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ac1x60vto1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1hpwhqt</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>NYE mani by me :)</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6gq5k1mo1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1hpw8tn</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying something new! </t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpw8tn</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1hpwdza</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting acrylics and I love them 😍 </t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpwdza</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1hpw5e3</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Today is a sad day. </t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6n1lmtwl1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1hpvokh</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Result of not cleaning underneath the nail </t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpvokh</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1hpvkx6</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Icicle/transparent nails ❄️✨</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpvkx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1hpvet8</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>idk what to do</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpvet8</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1hpvdvv</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple blue for nye </t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpvdvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1hpvc62</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Happy New Year</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/stz2lkspf1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1hpv319</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Tips for stubbornly dry cuticles?</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hpv319/tips_for_stubbornly_dry_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1hpv0q0</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Pretty 🩷</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwn254ccd1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1hpv01y</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>UV soft/gel bubbled up</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpv01y</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1hpuomx</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Hello Kitty Christmas Bauble set!🎄💕</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6fgpj1sa1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1hpujn7</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>The claws</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uojxjwmr91ae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1hpu8z0</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Wintery Glitz</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zr3lynxj71ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1hpu6hk</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Gel X removal question</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjt9x1a171ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1hpu1bm</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>NYE Nails!</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpu1bm</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1hptgi5</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>My nails for new years 😊</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hptgi5</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1hpted2</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Icy Claws 🧊</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bj3piti511ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1hpszi9</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>First ever manicure!</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpszi9</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1hpsji7</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Ready to start the new year with new nails</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2sb2knplu0ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1hpsb9m</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>New year’s vibes…..</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qcogsews0ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1hps75t</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black matte French with glossy tips </t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zrjfdnp1s0ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1hps6lp</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Forgot to post my holiday nails here 💚❤️</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hps6lp</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1hpjowu</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Press-on leftovers</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hpjowu/presson_leftovers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1hprvvb</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Sparkly NYE nails!</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hprvvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1hq99jw</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Clionadh &amp; Sassy Sauce hauls</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq99jw</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1hq996f</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>nail randomly broke</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3isre46eu4ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1hq8kpl</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t xml:space="preserve">craziest indie brands? </t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hq8kpl/craziest_indie_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1hq8cxv</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Carly and my nails</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq8cxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1hq7k4l</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dam nail polish NYE Mani </t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq7k4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1hq78m6</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>We match 💖</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trryeml884ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1hq778c</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>NINE ZERO</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hq778c/nine_zero/</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1hq6frc</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Mega just makes me want to dance!! ✨💅✨  Happy New Year!!  </t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s4z4k0i6z3ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1hq5rlj</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Classic 🩷</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/keu0g2aut3ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1hq5m1h</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>I am mesmerized 🪲</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qj5uh59es3ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1hq5458</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>December polishes</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq5458</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1hq4t83</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Red Carpet LED Soft Gel</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hq4t83/red_carpet_led_soft_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1hq4ngh</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NYE nails </t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq4ngh</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1hq40fu</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Does anyone have Mooncat's River Styx and ILNP No Days Off?</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hq40fu/does_anyone_have_mooncats_river_styx_and_ilnp_no/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1hq3x54</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Oh, for Oz Sake OPI Nail lacquer. Cirque Colors Liquid Laminate top Coat. I love the strong blue shift. </t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq3x54</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1hq3i07</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I ran here as fast as I could </t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w52wu0ry83ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1hq2ync</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is this? </t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq2ync</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1hq2pz6</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>My New Year's mani! 🤩</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq2pz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1hq294d</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can someone compare? </t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hq294d/can_someone_compare/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1hq278w</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My best friend and I made each other a nail polish advent calendar! </t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq278w</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1hq1w0p</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>No spectacular, green might not be my color</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq1w0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1hq1nda</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>(Resolutions) Set In Stone</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31h8c3o3t2ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1hq1ec7</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Last Blue and Silver Mani of the Year </t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq1ec7</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1hq0ors</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>NYE Nails 🎆🎇</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq0ors</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1hq0ivh</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Was out of town when my Black Friday orders started piling up and came home to this glorious mountain of orders 🥹</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq0ivh</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1hq04uh</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I might be obsessed </t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hq04uh</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1hpzes8</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Magnetic (Mis)adventures</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpzes8</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1hpzczl</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>🥂 ILNP Opening Night skittle for NYE (minus Curtain Call, I decided to save that for its own mani). Three coats of each with Spotlight as a topper.</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpzczl</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1hpz6p8</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>My First Ever Proper Polish Haul Arrived Yesterday!</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpz6p8</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1hpynu8</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat Raven + Accents! </t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5p4gjdx752ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1hpye8i</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Polish Catalog/Inventory Begins!</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpye8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1hpy7uj</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>10 digits, 10 polishes</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpy7uj</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1hpy46x</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Had to do a GIANT nail chop on both hands (they were broken so it was necessary😭). Rest in peace to my long nails, they haven’t been this short in over two years</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpy46x</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1hpxqfc</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prickling fear </t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/et507348y1ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1hpxoz2</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Essie QDTC speed setter streaky?</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hpxoz2/essie_qdtc_speed_setter_streaky/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1hpwu62</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>dark green for nye 💚✨️ *contains gifted pr*</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpwu62</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1hpw89q</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First major polish order! </t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4fl0y8jm1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1hpvwdj</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Ethereal - Pearl Mysteries &amp; GWP comparison</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hpvwdj/ethereal_pearl_mysteries_gwp_comparison/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1hpvltr</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Obsessed with the ILNP Fairy Shimmer bundle 🤩</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9fu6qrsh1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1hpvigc</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Experience layering ridge filler and base coat for longer wear?</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hpvigc/experience_layering_ridge_filler_and_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1hpvfjt</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Thoughts on Clionadh Polishes?</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hpvfjt/thoughts_on_clionadh_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1hpuz6o</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Top coat for velvet magnetics</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hpuz6o/top_coat_for_velvet_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1hpuvkf</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>December nails 🩵</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpuvkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1hpukzk</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>“Lava Nostalgia”</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpukzk</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1hpudi6</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Winter favorites</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hpudi6/winter_favorites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1hpu98c</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Mooncat a midsummer’s dream</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpu98c</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1hptzxd</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just a fabulous toddler </t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52p6zjzn51ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1hptxcq</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LONG lasting manicure, traditional polish with gel?? </t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hptxcq/long_lasting_manicure_traditional_polish_with_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1hptfv9</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>can you put regular polish on top of a gel base coat?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hptfv9/can_you_put_regular_polish_on_top_of_a_gel_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1hptffg</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Culprit’s Charm is crazy reflective 🩷</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hptffg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1hpt8p4</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>New year’s nails ✨</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xfpqmxdyz0ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1hpsfew</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>I know it isn`t fancy or much, but I love my little stash! + project polish update</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iur1qk7st0ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1hpsarg</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Making my own press ons is so much fun 🙂</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/864px0iss0ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1hprxtv</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>How my nails looked most my life VS how they look today</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hprxtv</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1hpru4o</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ready for the New Year </t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpru4o</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1hprjw7</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>(PR) Winter Wonderland nails for Hanukkah ❄️✨</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hprjw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1hprczb</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Settled in for some cozy winter ready, but distracted by my super sparkly nails!</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/evv9we8kl0ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1hprbi5</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Is there a good has everything you need starter gel kit?</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hprbi5/is_there_a_good_has_everything_you_need_starter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1hpr3ju</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Norpsilocin finally arrived🎉</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpr3ju</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1hpqpt5</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>My new (third) Helmer!</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpqpt5</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1hpqc5b</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>NYE mani 🎉</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxmoyqstd0ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1hpq5m5</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Press on nails too curved but already on nail</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epkhak8fc0ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1hpo3pt</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>🧲🌈Magentic Gradient🌈🧲</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpo3pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1hpnwuk</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>ILNP Cityscape for NYE</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y971gp4ctz9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1hpnww6</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>I’ve failed at stamping SO many times now, so it’s officially nail decal time!</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpnww6</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1hpntey</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>HEMA Pleasing Purple is a pleasant surprise😱</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpntey</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1hpnn3n</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Not convinced about my new years nails. Opinions?</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpnn3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1hpnle6</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Ready for the new year 💅🏻</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpnle6</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1hpmz2n</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How is bluesky for gel polishes and UV lamp? </t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hpmz2n/how_is_bluesky_for_gel_polishes_and_uv_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1hpmkx3</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Finally!</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a45hevp4gz9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1hpm91d</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Feeling like the Queen of the Emerald City 💚</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m2ja2n1gcz9e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1hpkwka</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hpkwka/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1hpkag4</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>I think I found my one true love</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpkag4</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1hpk811</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Essie - Chinchilly</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9d6v780oy9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1hp41qm</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>ILPN - Deep Space</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nmemlm9du9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1hpir4j</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>New Year's Eve Nails</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpir4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1hpwhb6</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>NYE mani by me :)</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mck3lfxio1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1hq8cx3</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Has anyone used the MPN / YJMyujimi painting gels?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hq8cx3/has_anyone_used_the_mpn_yjmyujimi_painting_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1hq74rn</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Love my nails so much</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kyrl8cm474ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1hq6voa</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Rate my state spirit nails</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d908m5tm44ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1hq3kc8</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are some nail art IG accounts that only use lacquer? </t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hq3kc8/what_are_some_nail_art_ig_accounts_that_only_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1hq2uct</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">YAY OR NAY </t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79siyrb633ae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1hq1ob3</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Drawing all those squiggles were fun</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62u2vitbt2ae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1hq1lnv</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Using metallic gel</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hq1lnv/using_metallic_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1hpyinj</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Graffiti (handpainted on press-ons)</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpyinj</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1hpx8hn</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Love me some festive clients, what about you?!</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jwe70teeu1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1hpunca</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Hello Kitty Christmas Bauble set! 🎄💕</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/96vq3uxha1ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1hpugc3</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Winter Set❄️</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79lk3e4291ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1hpu072</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>I made this set for the end of the year for a client, it is the first time I use embossing</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpu072</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1hprgxz</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails for the new year </t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zq37wgohm0ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1hpq6td</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Iridescent watercolor </t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpq6td</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1hpofip</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>clean elegant blue and gold nails 💠 kids are scary cause why did my 11yo niece ask for these.</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hy2hut2zwz9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1hpmuwy</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Gengar Nail Art</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpmuwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1hpkfr1</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Leopard Kitty!cute!!</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2axhqrnqy9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1hpkfdt</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hi Everyone.i am new on redit.here’s a picture of my newly done acrylic 3d nails.Feedback please </t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ic8dyo3oqy9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1hpjj4o</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried to paint a scenery </t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3q01zyt2fy9e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1hpin4o</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Yellow Holographic Cat Eye</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hpin4o</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jan  1 08:10:42 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_05.xlsx
+++ b/data/collected_data/2025_01_05.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C498"/>
+  <dimension ref="A1:C718"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8899,6 +8899,3746 @@
         </is>
       </c>
     </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1hqxisk</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqxisk</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1hqx43b</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Nails in 2024</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqx43b</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1hqx3g8</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>New Year's Eve Nails</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqx3g8</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1hqx350</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqx350</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1hqx2sj</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupe for OPI goldeneye? </t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1ufgs7aqbae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1hquro4</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Gel allergy…HEMA free safe?</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hquro4/gel_allergyhema_free_safe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1hqvj8t</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Gel allergy…HEMA free safe?</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqvj8t/gel_allergyhema_free_safe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1hqvrd8</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>A little late but my nail tech killed my Christmas set!</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqvrd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1hqvs5u</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Poetic justice NYE</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kmg5pn6gabae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1hqvr9h</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Accidental gel polish dust inhalation?</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqvr9h/accidental_gel_polish_dust_inhalation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1hqvbwq</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>First time doing dip nails with extensions at home....</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqvbwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1hqtw0b</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>extra wide nail tip recs??</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqtw0b/extra_wide_nail_tip_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1hqsmzi</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Heartbreaking start into the New Year</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqsmzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1hqtl7f</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>just got my nails done, are they supposed to look like this? my nail tech said they pointed up because of the shape of my nail bed, but the nails i had on last week weren’t pointed up like this :/</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqtl7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1hqtht5</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Wicked OPI GelColour</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqtht5/wicked_opi_gelcolour/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1hqtekv</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder Gels </t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqtekv/builder_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1hqte0d</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Back at it again! </t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bc5h0y0liaae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1hqtd9g</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>First time trying a colored french tip! Thoughts?</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://imgur.com/hikDyRt</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1hqs98p</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NYE nails! First time using cream gel. </t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2xf28pg6aae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1hqs8lh</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NYE Nails 💅 </t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7j2u5d096aae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1hqs5kq</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Finished Painting The Snowman and Irn bru boy for my Irn Bru Festival Nails! 🥰</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8a307a1f5aae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1hqrie8</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>New set for the new year! But have some questions…</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqrie8</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1hqq1el</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Really proud of my nail growth! First time doing a natural look with gel </t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqq1el</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1hqrjhg</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this acceptable work? </t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vj9n0hj5z9ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1hqr9ba</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Post holiday press-ons</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqr9ba</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1hqr2nn</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Can you spot the fakes?</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqr2nn</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1hqr2iv</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>I need a teeny tiny brush and I'd like one of those brushes that help with gradients. Where do I buy them?</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqr2iv/i_need_a_teeny_tiny_brush_and_id_like_one_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1hqr2ej</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Purple for New Years!</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zllyf3xeu9ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1hqqp5u</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Years Nails 🪩 </t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/59e7z6wnq9ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1hqoveb</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Engagement shoot nails/ First Manicure (update)</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqoveb</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1hqpbvs</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024 nails! </t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iaeqmu29d9ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1hqp8pz</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>How is this shape?</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbwmtxufc9ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1hqp73b</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fav sets I did on myself this year </t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqp73b</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1hqp2s4</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Dark chocolate square matte w glossy french tips</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f345pcqxa9ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1hqoxkf</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this nail shade clashing </t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqoxkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1hqoxj3</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painter’s antidote </t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpgxy9ok99ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1hqon4m</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Teal Glass</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3thsdzbv69ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1hqolz1</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving my new set! </t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqolz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1hqoi4b</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>first time using blooming gel!</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqoi4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1hqo8rc</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>gel pink pedicure</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbkboqs639ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1hqo6b2</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Is there a way to train nail beds to be a better shape?</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqo6b2</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1hqo61f</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail kit exploded </t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqo61f/my_nail_kit_exploded/</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1hqnbhd</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 💅🏻🎀🖤🎆🪩</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzbrybdvu8ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1hqmxb0</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>i’m a 17 year old licensed nail tech, all freehand!</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zngqbrz9r8ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1hqm9fu</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Taylor swift MTV outfit inspired nails</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/of0qvhwfl8ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1hqmeyn</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Acrylic beginner— how to prevent acrylic powder hardening in bowl?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqmeyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1hqmno9</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Pretty happy with how my dominant hand turned out (inspired by nailfocus1 on ig)</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqmno9</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1hqm46n</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Client nails that I did yesterday to close out 2024</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqm46n</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1hqlxch</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>How to make soft gel press ons (if possible)</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqlxch/how_to_make_soft_gel_press_ons_if_possible/</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1hqlgn9</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>I feel like I just got scammed at the nail salon.</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqlgn9/i_feel_like_i_just_got_scammed_at_the_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1hqlsz3</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Is this a good shape for me?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sozwuacfh8ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1hqlqi5</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t xml:space="preserve">False press ons - and a thank you  </t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dal96uitg8ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1hqlohw</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New year, new nails </t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqlohw</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1hql23y</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I know my thumbs are fat &amp; ugIy but cmon… the right one is DISGRACEFUL </t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rebv30h9b8ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1hqkovj</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Did Gel X for the First time! Feedback?</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqqypki588ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1hqkilg</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry Mocha gold butterflies </t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqkilg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1hqkfj7</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>NYE nails! ✨</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqkfj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1hqk2ns</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye NYE realness </t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rmqqmhz28ae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1hqk1us</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ending 2024 with my chipped nails </t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqk1us/ending_2024_with_my_chipped_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1hqjzow</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024 Recap </t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hubnuj928ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1hqjw3a</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Oval or square on my hands?</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sy7cw7ag18ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1hqjpg7</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>my first ever set of acrylics!</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e988ek8xz7ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1hqiq3d</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Ok so the nail tech RIPPED my acrylics off??</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqiq3d/ok_so_the_nail_tech_ripped_my_acrylics_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1hqj7t1</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Magenta chrome nails for vacation 🌺</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqj7t1</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1hqivlk</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Grape chrome</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqivlk</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1hqitcp</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>gifts for nail techs?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqitcp/gifts_for_nail_techs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1hqik3b</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Gel nails not setting</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqik3b/gel_nails_not_setting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1hqii9l</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Cuticle healing journey begins</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5tqzaqxp7ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1hqig35</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>New Year Nails✨️🎀</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqig35</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1hqhw4j</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Random question, the nail techs I always go to has the prettiest jewelry, always so shiny! Where do you think they get it from? </t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqhw4j/random_question_the_nail_techs_i_always_go_to_has/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1hqay89</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>HELP 😭</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n5mruy6lg5ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1hqc9xg</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>What to do about pinky toe nails?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqc9xg/what_to_do_about_pinky_toe_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1hqf6xi</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nail lifted and i can tell there's water under it! </t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqf6xi/nail_lifted_and_i_can_tell_theres_water_under_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1hqgx5g</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Speechless</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/az0xi4klc7ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1hqhlm8</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Mini lamps necessary?</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqhlm8/mini_lamps_necessary/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1hqhizj</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>The set I made for the holidays</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqhizj</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1hqha3l</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Do my nails look okay for the 3rd time doing them?</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqha3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1hqh8l9</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>purple lotus</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9lr6xc8cf7ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1hqh8bz</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>New 💫</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/st78x39af7ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1hqgynw</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Where can I buy this??</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqgynw</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1hqgizq</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>gold chrome going into 2025 🥳</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqgizq</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1hqg6pm</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Move over December's X-Mas nails, time for Winter themed nails in January! Done by me</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9klhit567ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1hqg46t</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t xml:space="preserve">holo to the new year! </t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ojjyoavd57ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1hqfezp</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Color changing sparkly pink 🥰</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66t8jvkxy6ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1hqf8fj</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Brown finger tips</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqf8fj</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1hqeomy</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Ending 2024 with this set 😍</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3xg7gdmr6ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1hqea2g</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Made my new years set </t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqea2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1hqe3gs</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>added some rhinestones ☆</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ga97ce9l6ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1hqdz1j</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New year's nails </t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bs4zoahvj6ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1hqdt8e</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>🎉 New Years Nails 2025 🎉</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzoylmvyh6ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1hqdn25</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>My new manicure - I think red is the color of passion</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpy8ddppf6ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1hqcxv6</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>It’s 2025 here in New Zealand, so…</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqcxv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1hqchyj</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Pink mermaid sparkles for new years! Made by me.</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/74o6dr1k16ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1hqcg7x</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>first time doing plastic extensions on myself + jelly polish + iridescent chrome powder+ ♡</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5v11fkt016ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1hqc6id</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry nails </t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqc6id</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1hqc3lg</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>My first French manicure.</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3ieyy5cw5ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1hqbf1w</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>My birthday nails!</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqbf1w</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1hqaxf9</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>First set of nails I tried to do for myself (press-ons with nail polish)</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqaxf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1hqaevn</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>naturals nails</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqaevn/naturals_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1hqy0b6</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm seeing the new Nosferatu film tomorrow, so I decided to paint the 1922 poster art on my nails. </t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqy0b6</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1hqxehn</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first homemade polish! </t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqxehn</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1hqwvfl</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>This mani survived a traumatic 24 hour labour with only tip wear</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yj5ihckqnbae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1hqwsyw</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Lurid lacquer - disquieting calm</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqwsyw</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1hqwmwy</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>December roundup</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqwmwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1hqwed5</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Fresh for the new year</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vq1uz0kshbae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1hqvkf8</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LyNb I Scream Sea over Cracked Chocolate Gram </t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqvkf8</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1hqvj26</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>The Return of Light</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqvj26</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1hqvduw</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Trying out the metal bracket horseshoe magnet dupe</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqvduw</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1hqvay4</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>✨NYE nails✨</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqvay4</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1hqv8gl</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How it started... How it ended </t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqv8gl</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1hqv3iv</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NYE Nails </t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqu7r5</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1hqv04z</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>I made a “holder thingy” for my wife’s nails as well as a “tray thingy” to slide into her UV lamp. All with built in magnets!</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9cqint801bae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1hquyvd</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The polish I chose for sitting on my couch tonight </t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9tikus1m0bae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1hqux6m</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone able to guess which nail has *resolutions* for the new year? </t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqux6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1hquuwh</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying out some toppers over my new blues I picked up before repainting them all solid blue and thought it might be helpful for someone💙✨ happy NYE!!! </t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hquuwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1hquhs6</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy New Year, Laqueristas! </t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hquhs6</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1hquh5b</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>I love the finish of this polish! Any suggestions for similar style, new color?</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hquh5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1hqu97e</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>introvert's NYE</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqu97e</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1hqu1kl</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Nail Chipping</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hqu1kl/nail_chipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1hqtxlr</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Loveliest polish I’ve ever used</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqtxlr</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1hqtfnc</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Sustainability and Beauty: Can Eco-Friendly Nail Products Lead the Way?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hqtfnc/sustainability_and_beauty_can_ecofriendly_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1hqtea4</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>New Year's Mani 🌠</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqtea4</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1hqtcf1</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Happy New Year</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqtcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1hqt7x0</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Wrapping your tips!</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqt7x0</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1hqsszj</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>American Apparel Nail Lacquer</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkymlpzacaae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1hqsp8q</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>An homage to the *best* Jelly Belly flavor</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqsp8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1hqshzc</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Adding my “Last Mani of the Year” to the mix. One last hurrah before a big chop to start the new year!</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqshzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1hqsbd9</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>My new years nails!</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98nqvwh37aae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1hqs9eg</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t xml:space="preserve">House of Hades for the last mani of the year </t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqs9eg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1hqs91c</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t xml:space="preserve">House of Hades for the last mani of the year </t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqs91c</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1hqs5q5</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>NYE nails 🥂🪩✨The future is a curious creature</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rw0j8tnm3aae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1hqs0g9</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Started in March of this year…</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqs0g9</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1hqrtr7</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Black and Gold NYE mani</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5gxvmjoy1aae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1hqrd5h</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Happy new year everyone!</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vmulkujcx9ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1hqr541</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>For New Year’s I decided the only way to start the New Year was by defying gravity 🎶</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqr541</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1hqr1h4</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>I could cry right now</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqr1h4</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1hqqqos</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Psilocin - deserving of ALL the hype</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqqqos</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1hqqjz8</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>What I wore in December</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqqjz8</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1hqqhhx</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>December manis🩷</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqqhhx</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1hqqcat</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>My new years nails</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqqcat</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1hqq6si</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>quick matte topcoat comparison</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x2073o6fl9ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1hqpy50</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Something Else by DVN</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqpy50</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1hqpvnl</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Favorite Obnoxiously Bright Lacquers?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hqpvnl/favorite_obnoxiously_bright_lacquers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1hqpt0e</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>🪩HAPPY NEW YEAR✨🥂✨</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88qadtouh9ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1hqpnyf</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Year’s resolution: more skittles? </t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqpnyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1hqpnvp</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>NYE Skittle 🪩</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqpnvp</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1hqpfs8</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>very impressed by the wear!</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vrvgvcxwd9ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1hqpezy</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>The New Year’s Nails</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rlvb5s64e9ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1hqpecf</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Is anyone tempted to try their nailspo?</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqpecf</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1hqp3rx</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Not very NYE</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqp3rx</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1hqoq43</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Ethereal’s Candlelight for NYE</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1nhs342n79ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1hqobgu</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>A nail polish that won’t irritate onycholysis?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hqobgu/a_nail_polish_that_wont_irritate_onycholysis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1hqo5ta</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Almost all of my swatching is done!</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2ph22jf29ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1hqnxd2</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone have recommendations for a good rubber base? </t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hqnxd2/anyone_have_recommendations_for_a_good_rubber_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1hqntko</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Champagne NYE Mani 🍾 </t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqntko</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1hqnnh0</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Fill in the blank!</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hqnnh0/fill_in_the_blank/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1hqnndj</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>NYE nails (also, photo tip for any NYC lacqueristas)</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zd5zj5iux8ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1hqnbv9</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>My NYE Nails + Seeking Help on how to Avoid Bubbles</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4op6skowu8ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1hqn6f5</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Happy New Year's ✨</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqn6f5</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1hqmcxt</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Appreciation post for all you beautiful laqueristas! </t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqmcxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1hqma5b</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>I’m too pretty to mess with</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqma5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1hqm8ss</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Gold tip lazy hack win ✨</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqm8ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1hqm7sw</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>3 hours after getting them done. I hate OPI</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/468ewec1l8ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1hqlw4n</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>my year in nail polish 🥰</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqlw4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1hqlmid</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New year, new nails </t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqlmid</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1hqlkko</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Allergies: the glue or the nails?</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hqlkko/allergies_the_glue_or_the_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1hqkvuk</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Created my first press-ons for NYE!</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65wav40t98ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1hqksk1</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t xml:space="preserve">december mani round-up </t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqksk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1hqkpek</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new year celestial cosmic 💫 </t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3zvsglk888ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1hqkls1</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A sad way to ring in the New Year! </t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqkls1</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1hqke6a</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Over filed a nail.</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hqke6a/over_filed_a_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1hqk4ga</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>NYE Manicure</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqk4ga</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1hqk3c1</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Solo Mission is gorgeous!! thankfully fending off all the raw meat allegations 🥩🫡</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqk3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1hqjtal</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Custom drawer pulls for Helmer</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ww6202r08ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1hqjqn5</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I get the hype </t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqjqn5</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1hqjom6</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>I basically chose flaky Wildberry Poptart for ringing in the new year.🤭😁</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ezpzb0qz7ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1hqjixu</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Asked coworkers for colors and they said purple and lilac 💜</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqjixu</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1hqj6yv</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Accidental Hershey kiss nails</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqj6yv</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1hqivie</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>NYE manicure!! ✨🔮 and shoutout to the ILNP team</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqivie</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1hqif9k</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cursed pose for ILNP Midnight Kiss 💋 </t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqif9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1hqhx0h</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Got some ILNP polish for Christmas and I’m obsessed!</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4xr1dc2l7ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1hqhp4a</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>(PR) Pomegranate nails for Hanukkah ❣️✨</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqhp4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1hqhorm</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Endlessly trying the most saturated blues I can find. What should I try next? 🔵</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqhorm</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1hqhnht</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Years Nails 🪩 </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6ku5yrhui7ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1hqhlsm</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Wasted my money</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3mowmihi7ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1hqgsnt</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>december’s nails 💅 goodbye 2024!!</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqgsnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1hqgqqx</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>My nails for the new year</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqgqqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1hqfzpf</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Velvet swatches using the new ILNP horseshoe magnet 💅🏼🧲</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8fi412la47ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1hqfki8</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Wintery for New Years!</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zxzriwxb07ae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1hqf6gw</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Let's see your new years nails</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqf6gw</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1hqewhy</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A year of nails </t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqewhy</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1hqeemf</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>NYE nails as inspired by redditors</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hqeemf/nye_nails_as_inspired_by_redditors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1hqe290</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Big sparse asym silver flakes topper</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqe290</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1hqdz7a</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Fallen angels</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqdz7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1hqcl88</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>NYE at the beach</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqcl88</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1hqci6d</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It even looks good on shortie nails! </t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqci6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1hq0w4t</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie gel x-I just got my nails done and this is the situation by the time I am home.Did I not dry it long enough? </t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15q4jyzzm2ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1hq8dqb</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I achieve this look without using gel? </t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khlowy97k4ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1hqavu4</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t xml:space="preserve">❄️ snowflake mani❄️ </t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqavu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1hqvxbj</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>NYE Nails!</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52f9xyc6cbae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1hques2</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>nye nails</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ucngj203uaae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1hqs6o7</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>🎇New Year’s Eve nails 🎆</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b9ygjnbq5aae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1hqs57v</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Finished Painting The Snowman and Irn bru boy for my Irn Bru Festival Nails! 🥰</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/df0m1o7b5aae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1hqnhd2</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>New Years nails🎉🥂💕</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7giux02dw8ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1hqms91</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>The start of a Ren and Stimpy set I’m practicing with</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zuoeddu0q8ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1hqml6o</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Fine Detail Brushes</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hqml6o/fine_detail_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1hqmh99</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Sonic</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lc00u3cn8ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1hqm71c</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>What do you do for brush control training?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xf8plmjuk8ae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1hqlfwl</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Bonnaroo Nails</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tidyxobhe8ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1hql0ci</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>2024 Recap</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fggoyv1va8ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1hqju3c</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Happy new years eve 🎆😊</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqju3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1hqja5c</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy NYE! </t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yc63y94cw7ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1hqi9dt</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are your nye nails? </t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zutmu5wn7ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1hqgkag</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Last set of the year</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqgkag</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1hqg0ob</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Christmas sets for this year 🥰 I know I’m late lol </t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqg0ob</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1hqe56w</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Palette cleanser from festive</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqe56w</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1hqe36i</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>what are your favourite unortodox nail art materials? (ei: watercolour, markers, etc)</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hqe36i/what_are_your_favourite_unortodox_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1hqdtfg</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>🎉 New Years Nails 2025 🎉</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4lo0r371i6ae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1hqbkzv</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>First time getting nails this long, and I absolutely love them! Nail art by the amazing Kimmy.</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqbkzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1hqaucg</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Spiderman and Venom</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hqaucg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jan  2 08:10:47 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_05.xlsx
+++ b/data/collected_data/2025_01_05.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C718"/>
+  <dimension ref="A1:C898"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12639,6 +12639,3066 @@
         </is>
       </c>
     </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1hroup8</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Wasn’t sure about this set at first but I think I LOVE them</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hroup8</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1hroiro</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Starting the new year with a fresh manicure! 💅</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hroiro</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1hrnlrt</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nuance nail art journey </t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrnlrt</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1hrnaqd</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>What nail color just screams I am DTF?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hrnaqd/what_nail_color_just_screams_i_am_dtf/</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1hrn8mo</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some glitters </t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrn8mo</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1hrm75w</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Please help me troubleshoot my gelx nails!</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hrm75w/please_help_me_troubleshoot_my_gelx_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1hrmfi9</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Caribbean vacation nail process! Scroll to see end result 😊</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrmfi9</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1hrmfcc</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My New Year's set! </t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrmfcc</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1hrm5mv</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>New Years Nails! What do you think?</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrm5mv</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1hrm34l</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>rubber base?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hrm34l/rubber_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1hrm2w4</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>My set for the New Year 💅🏾</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhqrgka4iiae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1hrlj1j</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Art Deco cat-eye nails hand-painted by me. Happy New Year! 🥂✨</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrlj1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1hrli93</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Nail tech re-envisioned my 13 y/o nail art</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrli93</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1hrlhkk</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Camilla as Stained Glass Painting Nail Art!</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrlhkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1hrkpoh</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Been practicing gel nails and nail art </t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikfokn4b4iae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1hrkn48</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using Kiss Press On Nails. Lucy and I are impressed.  </t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgy04vwl3iae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1hrka7k</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Prioritizing self care this year</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrka7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1hrjrlx</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Nails are lush..my wrinkly fingers not so much:(</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yolgoudmvhae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1hrjgbm</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any tips for securing nail? </t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4su2bmsnshae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1hrjdhr</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t xml:space="preserve">did my own acrylics for the first time and 4 popped off in 3 days </t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qabqksqyrhae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1hrjcrj</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>I know I'm late but here's my Christmas spirit 🌲🎅</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a50et8jhrhae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1hrjbnj</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NYE Nails! </t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qc3aqyahrhae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1hrhssv</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Fast drying nail polish</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hrhssv/fast_drying_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1hri7aa</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>will builder gel make my nail weak?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ht09zvodhhae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1hril44</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Press on sets I made!</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hril44</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1hri4gf</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My New Year’s Nails. </t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hri4gf</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1hrhbbt</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>New Years nails🎊🍾🥂💅🏼</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68yyj69k9hae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1hrgk6y</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Diy new years nails </t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0jq17433hae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1hrgjyp</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday NYE nails by @Hailssnailsss </t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83k7e4c13hae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1hrgh5c</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>New Year's Nails 💅</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrgh5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1hrgf83</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Winter Vibes</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrgf83</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1hrft9w</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>My NYE set</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9yayuvrwgae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1hrfs28</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Just did my nails (before the stones)</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/es99nevhwgae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1hrfd7z</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>My favorite nails yet!</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3goy3fqzsgae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1hrfcs4</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Sally Hansen "Holo-Back"</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrfcs4</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1hrezwq</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Losing specific nail</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hrezwq/losing_specific_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1hrdm8a</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>How to remove gel?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ben44egvegae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1hrek3k</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>I've been having fun doing my own nails lately☺️💅🏼</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrek3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1hrdy5d</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new years nails </t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrdy5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1hrdvxs</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Found this insanely packed Holo glitter polish in a bargain store for £1.50</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrdvxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1hrdlr0</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>First time doing gels at home!</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8oj2alregae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1hrdcht</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Loving this color (Sandviper by Mooncat)</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrdcht</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1hrcq44</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Grew out my nails &amp; started getting them done! </t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmezz93u7gae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1hrcmkw</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Nail Color Advice</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrcmkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1hrchoa</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>From Christmas to New Year’s Nails!</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrchoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1hrcheg</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>New Year Nails!</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrcheg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1hrce6r</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Entering 2025 🤩</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwy7hg775gae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1hrc5oa</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>New year, new nails</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jyph6oa3gae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1hrbttl</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Happy New Year! 🌌</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/casl81tm0gae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1hrbekg</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So pretty I can’t wait for my next set </t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0qec5h6xfae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1hrbbk4</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>First attempt at using sculpting gel!</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j128nk9iwfae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1hrb7lv</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Why did this happen?</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrb7lv</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1hrb7aw</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Happy New Year!</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rnjmpychvfae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1hr8vvs</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>dali nails + inspo</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr8vvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1hramo7</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail journey ✨ </t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hramo7</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1hr9r30</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>My (Unintentional) Glinda Set</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr9r30</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1hr9k08</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Press ons are awesome 🐲🐍</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr9k08</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1hr9iwn</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy New Year 🎆 </t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6l16g9hifae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1hr9h3k</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Builder gel</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2hacae13ifae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1hr99gp</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Never had my nails done before. Any advice on what I should ask for/get!</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hr99gp/never_had_my_nails_done_before_any_advice_on_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1hr97xb</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>HNY’s nails</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr97xb</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1hr8z5p</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Happy New Year 🎄</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7tbq1yk8efae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1hr8tic</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love this colour </t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ukuihszcfae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1hr6jnf</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>ive accidentally buffed/filed my nails too much.</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hr6jnf/ive_accidentally_buffedfiled_my_nails_too_much/</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1hr8gip</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Alt nails</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr8gip</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1hr8oon</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New year new set for the bestie </t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72zfwsaxbfae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1hr3ud9</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>How should I handle my next manicure with this broken nail?</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr3ud9</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1hr8bjn</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Peeling of gel nail polish </t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hr8bjn/peeling_of_gel_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1hr89sk</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Is there any way to avoid this</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr89sk</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1hr812o</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Tell me all your favourite/best products!</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hr812o/tell_me_all_your_favouritebest_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1hr7v79</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>New year, new nails</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr7v79</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1hr7lr7</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>it's past Christmas but idk if I showed off my holiday nails yet 🎄🎁</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ex377l7f3fae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1hr7ku9</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hand painted 2024 vs 2021💚 </t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr7ku9</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1hr7gd3</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has anyone bought anything from Sweeney nail supply recently and received their order? </t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hr7gd3/has_anyone_bought_anything_from_sweeney_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1hr7992</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr7992</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1hr6jj2</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Started getting my nails done </t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr6jj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1hr6ari</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Hi guys! How much should I be selling my Press ons for??</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ea2nbpzoseae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1hr5w3b</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Worst (and most dangerous) pedicure of my life. How can I speed up the healing process? Will my nail beds ever come back from this?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr5w3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1hr5lzu</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Is there a way to take press-ons on and off throughout the day?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hr5lzu/is_there_a_way_to_take_pressons_on_and_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1hr5aop</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>A simple &amp; clean start to the new year 💙🩵🤍</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr5aop</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1hr4u7b</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New year, time for new nails. Any suggestions? </t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8amjowvfeae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1hr2jan</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NYE At-Home Manicure </t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yurn68yzrdae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1hr2e5l</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is causing this? </t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5g2pk1ucqdae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1hqy3k2</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>I have thin, brittle, slow growing nails. Help!</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hqy3k2/i_have_thin_brittle_slow_growing_nails_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1hrnnee</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Thank you!! 💕💅🏼</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kr29a7wqziae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1hrnh1n</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Nails from MNF</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrnh1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1hrn84p</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Dupe for Wet n Wild 415a?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hrn84p/dupe_for_wet_n_wild_415a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1hrkpp5</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kbshimmer is having a liquidation sale. 20% off polishes that will be discontinued! </t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/htqq6q8b4iae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1hrkjr2</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Absolutely mesmerized by Deep Space </t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrkjr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1hrjjjx</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Confused about the light needed for DND gel polishes</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hrjjjx/confused_about_the_light_needed_for_dnd_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1hrjfu7</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Early birthday nails 💅 </t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrjfu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1hrjfsa</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Questions regarding DND gel polishes</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hrjfsa/questions_regarding_dnd_gel_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1hriwnt</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>My new favorite plum…</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8rzpfolnhae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1hrignp</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Looking for tips and tricks on improving my application technique</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hrignp/looking_for_tips_and_tricks_on_improving_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1hrifkt</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another win for sassy sauce 👏 </t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2fpufwofjhae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1hriagr</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>What color is champagne?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hriagr</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1hrhfms</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Does anyone use a bottle holder/stabilizer while they paint?</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hrhfms/does_anyone_use_a_bottle_holderstabilizer_while/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1hrhdiq</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I know my short nails are not the norm on thus sub, but I bought my first HOLO TACO polish today (color is Blue Rizzler) and I am OBSESSED with it! </t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5x9ecce2ahae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1hrh2z9</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My christmas gift! First time trying mooncat and I am in love </t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrh2z9</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1hrgylp</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2025 nail tracker! </t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrgylp</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1hrgslo</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t xml:space="preserve">a fun new year skittle </t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrgslo</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1hrgmsl</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Recently had LASIK done which means no more scratching my eyes when removing contacts!</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5p0mmqyp3hae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1hrg454</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>The Holo Taco advertising fiasco be like</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6w12wg6dzgae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1hrfzb1</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Tortoiseshell</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrfzb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1hrfyui</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Perfect periwinkle! </t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrfyui</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1hrfv8v</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Year’s Eve floor confetti 🎉 </t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrfv8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1hrft4d</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ALL THE SHIMMERS! </t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4vhwizlqwgae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1hrfspe</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Top 24 of 2024</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hrfspe/top_24_of_2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1hrf4uo</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Got engaged while wearing Ether Dragon</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uobfphj2rgae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1hrduwm</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>December nails</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrduwm</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1hrdn73</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Going into 2025 with the Glory of Innocence feat. My dog </t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vl48a223fgae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1hrdkj4</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A feverish orphan with a soup deficiency </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrdkj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1hrd6ws</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Better Nails 2025</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hrd6ws/better_nails_2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1hrd3yg</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>akemashite omedetou! congrats on surviving to a new year!</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrd3yg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1hrd0pg</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Best peely base coat? UNT is very inconsistent</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hrd0pg/best_peely_base_coat_unt_is_very_inconsistent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1hrcwb5</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Glimmer ✨</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrcwb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1hrcthw</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It begins… </t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86pat89m8gae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1hrclye</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>My 2024 recap 🥂</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrclye</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1hrcgn9</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Thought these were more similar….</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mcbn23q5gae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1hrcfpr</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>What are your favorite polishes for gloomy days?</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrcfpr</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1hrcfbx</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Year’s Nails! </t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/braotmlf5gae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1hrcd6e</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>a very basic gold shimmer for the new years</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iv873okz4gae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1hrbyt0</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>New Year, New Chaos: Unboxing Pandora’s Box 💅✨</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7zha12o1gae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1hrbvts</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Organized my polishes for the new year!</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrbvts</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1hrbpnx</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Sparkly icy skittle for 2025!</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrbpnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1hrbk0n</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>I'm in love with this polish</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ed37rbadyfae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1hraks8</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>A happy side effect of Invisalign: I physically can’t bite my nails anymore!! Celebrating with my first ever jelly sandwich 🥪</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjwdtqolqfae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1hra815</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Getting a smooth polish line by your cuticles</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hra815/getting_a_smooth_polish_line_by_your_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1hr9t4w</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>December Manis ☃️</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr9t4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1hr9r42</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>New UV Lamp Needed: The Hunt?</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hr9r42/new_uv_lamp_needed_the_hunt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1hr9p4v</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t xml:space="preserve">anyone else in bed with their cats today? 😌 </t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr9p4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1hr9mm1</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>How to get polish application super neat?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8tidt4ajfae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1hr9lw6</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>What I wore as a skittle mani going into 2025! (ft my uneven nail lengths)</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr9lw6</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1hr9avf</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>💚Green for a fresh start to the New Year</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqc3sqergfae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1hr9aks</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Happy New Year everyone! Starting to work through my Christmas haul…</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hu2e3pyngfae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1hr99l5</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>New years mani</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr99l5</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1hr8yc4</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Added sparkly polish on top of my existing polish on a whim. Feeling very festive!</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr8yc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1hr8rs6</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>BKL Rat</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5ky8f53lcfae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1hr8o5c</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inspired by the end-of-year posts on here! </t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0csgdowsbfae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1hr8nu0</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HT Price of Alexandrite vs. MC A Most Destructive Melody </t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hr8nu0/ht_price_of_alexandrite_vs_mc_a_most_destructive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1hr8frb</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Final night of Hanukkah nails 💙✨ (Paid/PR)</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr8frb</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1hr82at</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Ringing in the New Year with a 💥BANG</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr82at</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1hr7l9x</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>OOTL on Squidbrains &amp; Crafted Hues recent split</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hr7l9x/ootl_on_squidbrains_crafted_hues_recent_split/</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1hr7f2m</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Happy New Year!!</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3z8vufw1fae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1hr7da0</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>I can't stop staring 😭</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s08twtjh1fae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1hr70h8</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Cassiopeia by Cirque Colors - my first magnetic polish 💜</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/idgsdn9kyeae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1hr6f5a</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>New Year, New Mani</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1iv1roaoteae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1hr65f3</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Small Cirque Colors order to start the year. Soleil was a surprise stand out. </t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zk27kb9greae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1hr629u</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Christmas/Nee Year Mani</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr629u</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1hr60b6</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Some of my favorites from 2024!</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr60b6</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1hr5ysw</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A Galaxy Far, Far Away is truly out of this world </t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/am9fw69xpeae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1hr5rwk</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The year of the manicure </t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bc3dz8aoeae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1hr56hu</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Okay these boxes are actually worth keeping (plus what was inside them)</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr56hu</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1hr5691</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Blue, purple, silver shimmer…</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr5691</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1hr4e2k</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Happy 2025!</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/jAmo2Is</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1hr4dn2</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>✨️🌈💅2024 Recap💅🌈✨️</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr4dn2</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1hr48db</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>2025 sparkles! ✨</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgd6trx6aeae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1hr2maz</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A moody new year mani </t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr2maz</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1hr23hf</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally tried Cygnus Loop </t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qph04hyjmdae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1hr1xza</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Ombre with gel polish ?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzpae4fpkdae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1hr1xz2</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Exactly 1 year ago, I developed a gel allergy. Here's a compilation of me relearning how to use and love regular polish.</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xp6mwjdkhdae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1hr1g83</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>In love with Catfished🩵</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p2h2ko5hedae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1hqx326</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Dupe for OPI goldeneye?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1p09p0jdqbae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1hr0upa</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hr0upa/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1hr0uek</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>I painted my nails for the first time in ages</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3jkaynad6dae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1hr0nc0</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>new years nails ✨</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr0nc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1hr0ky8</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm a magpie. </t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9iquwq7s2dae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1hqypbz</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Thinner didn’t work on polish?</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wzirp13racae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1hrljv1</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Art deco hand-painted cat-eye nails by me. Happy New Year! 🥂✨</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrljv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1hrli1g</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Camilla as Stained Glass Painting Nail Art!</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrli1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1hrl5ud</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute nails for new year </t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrl5ud</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1hrh6da</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Reusable way to clean clear jelly stampers?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hrh6da/reusable_way_to_clean_clear_jelly_stampers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1hrgm5c</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>christmas snoopy nail art by me!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okqkou9k3hae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1hrf6zh</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t xml:space="preserve">happy new years! </t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rs4opbpjrgae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1hresl6</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>My Christmas nails</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/areg434dogae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1hr9bc8</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Are they okay?</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1fvr515vgfae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1hr8q4m</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some 3D practice! </t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr8q4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1hr7bid</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr7bid</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1hr4uud</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One of my works, my own new years nails </t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5wix7c12geae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1hr241r</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Happy New Year!</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hr241r</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jan  3 08:10:52 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_05.xlsx
+++ b/data/collected_data/2025_01_05.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C898"/>
+  <dimension ref="A1:C1105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15699,6 +15699,3525 @@
         </is>
       </c>
     </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1hshhc0</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>My new set (by me) with some fake opals i made</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a3yodmd0kqae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1hsgnd6</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do these look too much like press-ons? </t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsgnd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1hsg39f</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>I thought it was impossible. I thought wrong ❤️</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsg39f</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1hsfc8t</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using nail polish </t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnzdu7pmupae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1hsfauv</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>I love this almond shape and this design</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37zxoh88upae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1hsf3ih</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Hiya!! Anyone with sensitivities?</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hsf3ih/hiya_anyone_with_sensitivities/</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1hsf6hk</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Disaster struck, advice</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hsf6hk/disaster_struck_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1hsf4z5</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need help communicating lack of symmetry </t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ngc9n3hspae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1hsf4u5</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>OPI "infinate shine 2" gel-like polish still smudging after 20 or so minutes?</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36yz6qnfspae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1hserw1</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>First set of the year! 🐚⭐️</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hserw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1hsenrw</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Winter Chrome ❄️</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5z9pf7onpae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1hsekmg</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Casual but elegant, yes or no?</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xgik5ygrmpae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1hsdofq</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Recommendation request!</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hsdofq/recommendation_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1hsd6fv</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Help! Can I use press ons?</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uy9dts389pae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1hsde9t</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>My favorite nails of 2024✨✨</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsde9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1hsdcgg</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails </t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5oi0t1uapae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1hsdaok</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>all Christmas nails I did for 2024:)</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsdaok</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1hsd9zn</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t xml:space="preserve">some recent nails : ) </t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsd9zn</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1hsd9k9</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Chrome blobs</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zv4b4li2apae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1hsd837</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New press ons! </t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hsd837/new_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1hsd10c</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Can I do 3D nail art with builders gel using regular, non gel polish?</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rggi70ot7pae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1hsce8e</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Does anyone know of any gel polish that would give me similar results as an Opal?</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsce8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1hscrj2</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>My new nail 🎀✨</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mx6u621d5pae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1hscbyc</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Press ons: How cheap is too cheap? How expensive is too expensive?</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hscbyc/press_ons_how_cheap_is_too_cheap_how_expensive_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1hsc8y4</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel c recommendations </t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hsc8y4/gel_c_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1hsc67o</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New to Gel-X - are they supposed to be so curved and bulbous? </t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsc67o</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1hsbs5w</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I loved them </t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8ip0famwoae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1hsbo7k</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i’m a 17 year old nail tech, all freehand! pt. 2 </t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsbo7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1hsbl9t</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024 nails wrapped </t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsbl9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1hsbj11</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t xml:space="preserve">honestly no one has me beat </t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l83ok37cuoae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1hsbevi</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Nail shape Yay or Nay?</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsbevi</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1hsbd28</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Loving Matte</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hsbd28/loving_matte/</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1hsb004</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>are my nails more almond or stiletto shaped? i asked for shorter stilettos but i kind of feel like these look more almond shaped. i’m curious to hear your opinions!</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myzh21stpoae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1hs8akv</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>How do I improve at taking nail photos?</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs8akv</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1hs9vgs</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>I REALLY NEED HELP</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/64x62msjgoae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1hsad0g</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>❤️👍</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ymzn7ewikoae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1hs9yrl</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Poor retention with Gel X</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hs9yrl/poor_retention_with_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1hs9s2i</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Midnight snowflakes painted freehand 🤯. The woman who does my nails is spectacular!!!!</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bm382tuqfoae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1hs9rrm</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New obsession unlocked </t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs9rrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1hs9mn2</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bling Nails! </t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs9mn2</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1hs9g8n</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Gel keeps coming off!!</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hs9g8n/gel_keeps_coming_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1hs9g6p</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>How to shape short almond nails?</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hs9g6p/how_to_shape_short_almond_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1hs921k</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t xml:space="preserve">she just told me “ I want green” </t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5yp2pf0aoae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1hs91id</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday Nails!! </t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hr286hcw9oae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1hs909q</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Did my own gemstone nails for the new year ✨</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs909q</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1hs8b9e</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Mint green and silver ✨</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs8b9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1hs7wi4</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They asked me to marry them! Luckily I had a fresh manicure 😄 </t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs7wi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1hs7sj7</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Press-On Brand with Extra Wide Sizing?</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hs7sj7/presson_brand_with_extra_wide_sizing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1hs7tex</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>What do you think of my new set?</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bsewjyr80oae1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1hs7iwu</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gamer girl nails </t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hx7gdgqyxnae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1hs7if8</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>beginning to now</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs7if8</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1hs6y92</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Kicking off 2025 with a sweet little French Mani.</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1k9vtzltnae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1hs6czs</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Decided to be a little extra for my first mani of the year…</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs6czs</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1hs68ud</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Nail shape</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hs68ud/nail_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1hs68gm</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>are these too thick?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs68gm</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1hs5fmn</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>nail looks dull</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hs5fmn/nail_looks_dull/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1hs577v</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Balatro inspired nail design</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs577v</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1hs599s</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>How long do your toenails have to be for a pedicure?</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hs599s/how_long_do_your_toenails_have_to_be_for_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1hs3k98</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Gels inc. BIAB don't stick to my nails</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hs3k98/gels_inc_biab_dont_stick_to_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1hs31ro</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Help with skin</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofhs5a5t0nae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1hs182t</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Winter colours/ design</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hs182t/winter_colours_design/</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1hs2vha</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t xml:space="preserve">anyone else extremely basic when it comes to thier nails? </t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3x4cbkkzmae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1hs2utq</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>My left thumb nail grows really flat with a weird divot at the</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs2utq</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1hs1vrt</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Does anyone know of a color similar to OPI You Sustain Me?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs1vrt</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1hs2abn</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>ILNP Trick or Treat</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ihjl98cvmae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1hs1t1d</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thoughts on this shape on me? </t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs1t1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1hs1p45</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Grown out but still very cute. 🖤✨</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs1p45</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1hs1n2n</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A year of nails! </t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs1n2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1hs1eer</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Fourth set I’ve done myself!</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mtfapakyomae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1hs1ayl</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cure for this? </t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zs5is6iaomae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1hs0z7n</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>first builder gel nail set – definitely a work in progress!!😬</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs0z7n</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1hs0kqn</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>cutest nails my best friend ever did on me 😍</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs0kqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1hrzydp</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone know a similar color? </t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kxgg7hiemae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1hs03ud</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Silver and grey</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs03ud</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1hs03kn</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>My birthday nails &lt;3</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs03kn</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1hrz6x3</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>I like to call this the Pregnancy/chronic illness manicure!</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrz6x3</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1hrz3q9</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got new naaaaiiillss </t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrz3q9</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1hrypcm</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>new year, fresh me. 💋</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrypcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1hrykq8</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Milky white nails 🪽</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrykq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1hryjmw</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Made these for a Press-On Collector</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jna978284mae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1hrxvz9</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>HELP! My nails keep breaking</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrxvz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1hrxr9u</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Rubber gel vs UV gel vs Builder Gel</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hrxr9u/rubber_gel_vs_uv_gel_vs_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1hrp440</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing nails </t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrp440</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1hrqe7m</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Will this become an issue? :/</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jrxb9glzjae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1hru8u9</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>I smashed my finger in a window. Do I call my nail tech?</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hru8u9</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1hrw95i</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>This one’s for u/wiscomama</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrw95i</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1hrvkgl</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Discord for learning about Nails</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hrvkgl/discord_for_learning_about_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1hrwzja</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Allergic reaction to top coat??</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4k4uxvssslae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1hrx0bh</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Why do my nails always look damaged like this after wearing nail polish?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2rot6kyslae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1hrwvp4</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Back to basics with my fave milky white gel DIY</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrwvp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1hrwogx</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Shelf life of some indie brand polishes?</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hrwogx/shelf_life_of_some_indie_brand_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1hrwm0l</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>New year, nails</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9p24ulkyplae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1hrvlrn</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Have you ever had an air pocket inside your nail?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hrvlrn/have_you_ever_had_an_air_pocket_inside_your_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1hrtkic</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Christmas nails vs New Year's nails</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrtkic</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1hrtawj</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone know what this could be on my nail? </t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4mwwxytxkae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1hrt9m3</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>What do you call these in english and can you remove them? How?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1kmg0phxkae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1hrsydo</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Press on nails and Mold</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hrsydo/press_on_nails_and_mold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1hrswmx</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>My base gel is leaking</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrswmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1hrsk90</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Keeping the Christmas spirit alive a little longer ✨</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrsk90</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1hrs7ta</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New year new nails!! 💅🏿 </t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrs7ta</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1hshh3m</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Tried a thermal, only for it to be too hot to activate at all, whoops!</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hshh3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1hsh1ty</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Sinful Colors 837 Shirley &amp; Buddy</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsh1ty</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1hsfa4q</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reminisce </t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsfa4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1hsf7oy</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel/acrylic alternatives </t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6te74z9tpae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1hsey74</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Mermaid Bait mesmerizing me</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsey74</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1hsexts</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>when you love your PPU shades</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsexts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1hsevsd</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>New years nails ✨</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsevsd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1hsetdi</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>kbshimmer question</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hsetdi/kbshimmer_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1hseit9</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>It's Only Forever</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hseit9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1hsdr41</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> I can sit still for two hours and once I move my manicure gets ruined 😭</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8r4yq5umepae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1hsd7bx</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>My first BKL! I am THRILLED！Look at her 🦊!</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsd7bx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1hscpna</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Icy goodness! ✨</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hscpna</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1hscafg</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! looking for a quick dry (no UV light) polish that looks like Gelcare Rose Water in photo below:  Everything I've found is not sheer enough... </t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hscafg/help_looking_for_a_quick_dry_no_uv_light_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1hsc38n</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Danglefoot It’s Glo Time as my first of the year</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsc38n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1hsau1j</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Yellow line near the whites of my nails?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n878bivhooae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1hsarri</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Bee’s Knees - Give it back tenfold</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c62yf4lznoae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1hs9sn2</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>I did the big cut.</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs9sn2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1hs9nsn</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Bling Nails!</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs9nsn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1hs89yj</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>ILNP Haul for 2025</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs89yj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1hs83j2</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bringing in the new year with a ✨silver adjacent✨ polish </t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs83j2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1hs80a6</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Been enjoying seeing progress pics so here's how my own shaping + photos skills have changed from 2021-2024</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs80a6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1hs74f2</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>I'm on a quest for the perfect opal mani. I'm not there yet, but I'm getting close!</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o48i6ekxsnae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1hs6yqz</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>three cirque reds</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hvfivpxitnae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1hs6ra3</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Show me your first mani of 2025!</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6im53yi5snae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1hs6lzu</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>To new beginnings!</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txrxvii1rnae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1hs6c1u</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>My NYE mani 🪩🎊</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs6c1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1hs671a</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Cock a doodle doom - sassy sauce</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs671a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1hs5w47</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t xml:space="preserve">thank you to this sub! </t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs5w47</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1hs5p5l</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Be Honest - Does this give “dead mannequin” vibes? </t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs5p5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1hs5ol4</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Small NYD haul </t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dosito6knae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1hs5oai</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>As I finally mastered the art of velvetizing, what magnetic polish is the best of the best for you? Which one did not live up to your expectations? I kinda want all of them now but ... you know how it is</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9es9px3rjnae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1hs5ikn</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Dupe?</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs5ikn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1hriweg</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>NYE nails</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cex8znnlnhae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1hrqphd</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Apres gel x alternatives</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hrqphd/apres_gel_x_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1hrwmve</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Shelf life of Indie Brand Polishes</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hrwmve/shelf_life_of_indie_brand_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1hs16c4</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Velvet Nails</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hs16c4/velvet_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1hs58f2</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Everything Swatched!</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5aajimtgnae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1hs4wup</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Kathleen &amp; Co restocking It’s Showtime!!!!</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs4wup</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1hs4qs7</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The ultimate purple </t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs4qs7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1hs4n11</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>ILNP Ariel</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2iwxm5fcnae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1hs4lgy</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NYE late post </t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02u2q7k6cnae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1hs3z8c</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Created a sponge gradient using psilo/psilo-siblings </t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs3z8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1hs3fz1</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Holiday Mani Round-Up!</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs3fz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1hs29qj</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>How to avoid nail salons that are bad for your nails?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hs29qj/how_to_avoid_nail_salons_that_are_bad_for_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1hs294m</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Glittering into the new year✨🪩</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lpqa6k30vmae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1hs1vxz</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Starrily's "Dragon" with Holo Taco's "Gold Flake Taco"</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cd40eqjfsmae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1hs1jmf</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A bit late but I finally got to see the movie 🪄🧹🩷💚 (contains products I've received as pr) </t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs1jmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1hs177c</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1x coat of Sweet Pea + a dash of feline </t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs177c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1hs12wv</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>I love Holo. ❤️</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zmdqeoulmmae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1hs0yos</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>First nails of 2025!!</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs0yos</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1hs0u2t</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>I was bored of my NY nails so I added some cracked gold</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efie3qfokmae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1hs0nsj</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>What I asked for vs what I got</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs0nsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1hs0n15</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>A bit late, but here's my NYE disco ball nails 🕺</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs0n15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1hs0dhp</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This blue is bright and eye catching!!  Essie’s  “butler please #772“ I love it! </t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs0dhp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1hs02u0</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Sixth Station ✨️</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs02u0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1hrzz29</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Bought myself my first "specialty" nail polish for Christmas, I fear I'm at the beginning of developing an expensive habit. Mooncat - curiosity's prey</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hrzz29/bought_myself_my_first_specialty_nail_polish_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1hrzmc3</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>My first ever ILNP, beyond obsessed!</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrzmc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1hryvkq</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Girlies what nail polish/powder should I use for Jinx's missing/mechanic finger??</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/as8pk4ng6mae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1hrynh7</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>cranberry vampy new year winter vibes mayhaps?</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrynh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1hryjnc</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>1st mani of the new year: Maelstrom</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hryjnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1hrygx6</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie - Forever Yummy! </t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrygx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1hry9dg</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Damaged nails from playing violin!!</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hry9dg/damaged_nails_from_playing_violin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1hry941</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Where to buy solvent resistant glitter</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hry941/where_to_buy_solvent_resistant_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1hrxyr6</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>HELP! My nails keep breaking</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrxyr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1hrxkvw</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Turbocharged Deep Space</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrxkvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1hrxknf</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I compared my wedding nails ('22) to my nails now and I'm so happy at my personal progress. </t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uq75mmb7xlae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1hrwwaj</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i think I grew my nail beds really nicely? </t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrwwaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1hrwstr</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>My new favorite polish, KB Shimmer "It's Fall Good" 🍁 ✨</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a373jfudrlae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1hrwlsd</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Silky start to the New Year</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7moo44gvplae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1hrw6l3</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>needless to say, i have a new adhd hyperfixation</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9puggalmlae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1hrw4im</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>A frosty shade to start off the year</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrw4im</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1hrvyis</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Help me choose between carts @ Garden Path, Mooncat, &amp; ILNP. Trying to stay around $80 or less.</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/asxwmuysklae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1hrvojp</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Okay, after this one I will stop annoying you all with Hex :D</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwy1ingjilae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1hrvmle</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Why are the prettiest polishes the most difficult to photograph? This is Lightwave ILNP (magnetic) and top and base coat is Sally Hansen Complete Care 7-in-1 Nail Treatment.</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrvmle</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1hrvd3n</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>sally hansen 3 in 1 QTC - thoughts?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hrvd3n/sally_hansen_3_in_1_qtc_thoughts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1hrva1b</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Plan to have baby </t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hrva1b/plan_to_have_baby/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1hrv8cb</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>ILNP Bluebell!</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrv8cb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1hrv08s</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>My nails come alive at dusk 🧚🏾🌅</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrv08s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1hrur3e</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can't wait for spring </t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6segttqxalae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1hrukdb</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Looking Up by ILNP topped with Everything Taco by Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrukdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1hrue2b</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>starting off the year with a classic: the ✨glazed doughnut look✨</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrue2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1hrt8cr</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Nail Polish Journal 2024</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrt8cr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1hrsvs0</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why do my nails keep splitting high near the nail bed when I grow them using builder gel? </t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrsvs0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1hrr805</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phoenix - Bella is so pretty I can't stop randomly staring and taking photos </t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrr805</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1hrpcva</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do the health concerns related to gel polishes apply to OPI Infinite Shines? </t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hrpcva/do_the_health_concerns_related_to_gel_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1hrpc2a</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>december 2024: i ended with HT + colores de carol</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrpc2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1hrp8ip</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>january 2024: i began with A england</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/em3pt8tvjjae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1hrp6bq</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Blade of the Frontiers for NYE</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5ipjbs4jjae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1hsh6cu</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Cybersigilism Miffy</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsh6cu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1hs6k4q</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My holiday nails! ❄️ </t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rckps0nqnae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1hrr1dj</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Space girl nails 💫💥</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6d2vxd58kae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1hsfdr5</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French reverse technique that did my manicure the other day! It's so delicate and pretty, I can't stop making this design again haha ​​it drives me crazy </t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzga8x73vpae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1hsdjyl</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>I know it’s late for Christmas but they are so cute</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsdjyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1hsc6py</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>First design to start off the New Year 🥂</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsc6py</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1hsawm2</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>How much would you say these are worth ?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsawm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1hs9pwe</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Bling Nails!</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs9pwe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1hs8mqj</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>They asked me to marry them! Luckily I had a fresh manicure</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs8mqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1hs1xyd</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs1xyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1hs02my</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Silver and grey</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hs02my</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1hrys6v</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>First set of 2025</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/npl3vk806mae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1hrxd62</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Christmas Set ft. my favorite brewery</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrxd62</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1hrx7en</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Fresh camo set</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrx7en</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1hrw6co</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is he a bit.... Voldemort looking? </t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sz2kl87kmlae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1hru04e</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Tried to build some acrylic nails with nails forms(any tips how i can improve?)</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hru04e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1hrqp44</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy new Year </t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvg023li3kae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1hrpray</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Throwback to Two of My Favorite Halloween Nail Designs So Far</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrpray</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1hrpe54</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Nail sets of 2024</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hrpe54</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jan  4 08:09:23 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_05.xlsx
+++ b/data/collected_data/2025_01_05.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1105"/>
+  <dimension ref="A1:C1320"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19218,6 +19218,3661 @@
         </is>
       </c>
     </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1ht99al</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Okay, honesty hour, besties—do these press ons fit my nail beds okay, or do I need to take them off and do some more filing?</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht99al</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1ht8fwz</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Ombré French Tips</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnkq4f879xae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1ht81ne</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Acrylic set ✨</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht81ne</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1ht7xyt</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>3rd set of nail art on myself</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht7xyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1ht76wi</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>My Nails 💓 Old pic I found. Do you guys think I should get these nails done again??</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7phz8eo9vwae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1ht79z9</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed </t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht79z9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1ht689d</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Which shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht689d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1ht66a7</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>What did my nail tech put on my nails??</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ht66a7/what_did_my_nail_tech_put_on_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1ht5scs</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>I need help please💙💚</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ht5scs/i_need_help_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1ht5q9m</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I am extremely happy with my new nails!!!! </t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht5q9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1ht5mfr</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>First DIY Gel Manicure French Chrome</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht5mfr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1ht5e5l</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Not new for doing my nails, but any recommendations for colors, patterns, or shapes?</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ht5e5l/not_new_for_doing_my_nails_but_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1ht5c11</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Any nail artist recommendations for Lunar New Year designs in Vancouver?</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ht5c11/any_nail_artist_recommendations_for_lunar_new/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1ht595h</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>First set of 2025</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdh7z9s4cwae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1ht54mq</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>My first time doing anything like this on my nails. Gel x, navy polish with chrome, 3D gel.</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht54mq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1ht4upy</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Is this UV light good enough?</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8aftf2c8wae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1ht4nnu</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Gel topcoat over powder manicure peeling... normal?</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ht4nnu/gel_topcoat_over_powder_manicure_peeling_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1ht4gcs</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Time for a change </t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gs8femtj4wae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1ht431v</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Chipped 2 nails opening a Mini Brands ball</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8ythdh21wae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1ht3lyi</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>the only photogenic part of me 🤎🐻☕️</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht3lyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1ht3khg</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Size 12?</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ht3khg/size_12/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1ht3dz6</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Help please guys.....</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ht3dz6/help_please_guys/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1ht36f4</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Picky allergy?</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ht36f4/picky_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1ht3cqq</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Starting the year off strong ✨</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhpnafniuvae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1ht38wo</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Help !!!</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ht38wo/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1ht32ho</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does using gel polish that doesn’t have to be cured still protect your natural nails?  </t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ht32ho/does_using_gel_polish_that_doesnt_have_to_be/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1ht2sn3</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Latest Nails!!</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht2sn3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1ht2c6t</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got an Olive and June gel kit and Led lamp as well as some madam glam gels for Christmas. Is it okay to use the madam glam polish with the Olive and June lamp? </t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ht2c6t/i_got_an_olive_and_june_gel_kit_and_led_lamp_as/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1ht2kcz</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>New set ✨</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmclk7hknvae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1ht2gf6</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does any1 know how to keep nails on longer? </t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ht2gf6/does_any1_know_how_to_keep_nails_on_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1ht1r0p</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing my own gel at home! </t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht1r0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1ht1gvi</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nails? </t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ht1gvi/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1ht1ms1</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Wintery Set</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/teuevj0rfvae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1ht175d</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Cherry Bomb 🍒💣</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hraux28cvae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1ht05gm</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Note to self: damaged, brittle nails and good prep do not go together </t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht05gm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1ht0ps2</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this all in my head? </t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ht0ps2/is_this_all_in_my_head/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1ht0xdi</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>First nails of 2025 setting a high bar!</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ht0xdi/first_nails_of_2025_setting_a_high_bar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1ht0dwu</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>new set of coquette nails 🎀✨</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht0dwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1hszzt3</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails </t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0xpedb1n2vae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1hszqjy</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New year sparkly spiderwebs </t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hszqjy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1hszfje</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Which nail tech did a better job? (Ignore the fact that one nail is mat and one is shiny)</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hszfje</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1hszf95</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Almost a year of growth!</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hszf95</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1hsz8gk</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time working with hard gel! </t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsz8gk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1hsz7qw</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Simple and clean</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsz7qw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1hsz6kq</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Do you need two lamps for at home gel x nails?</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rcl440oawuae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1hsyz69</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set of 2025 ✨ ☀️ </t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvgx5sxouuae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1hsydvz</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>I'm so scared of gel allergy so I'll throw everything away</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hsydvz/im_so_scared_of_gel_allergy_so_ill_throw/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1hsxiuj</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>What is this?</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2muozwpojuae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1hsy8d7</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Starting off simple ‘25</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trv15i20puae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1hsxr8t</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set of the year </t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsxr8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1hsx9mz</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Am I being unreasonable?</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsx9mz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1hswrjk</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>I recently started painting my own nails and wanted to show my latest one!</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oy2710zxduae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1hsw8n5</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Was met with a surprise tonight… my cat eye nails are glow in the dark!!! </t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ugid2jv9uae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1hsvpnx</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Can I build off of this? PLZ, I don’t have or feel comfortable using acrylics yet. My thumb nail is growin back pretty fast but it’s       Ew 😭</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uk9afudu5uae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1hsvf6f</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>New Nails for 2025!</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsvf6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1hsvdrl</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love Chinese pottery </t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsvdrl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1hsv13k</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Old porcelain inspired set (handpainted press-ons)</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsv13k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1hsv7ok</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is the gel used to set gel x nails the same as a regular uv/led gel, or is it a special glue gel you need to use? </t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hsv7ok/is_the_gel_used_to_set_gel_x_nails_the_same_as_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1hsugqt</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>What am I doing wrong for ballerina/coffin shape?</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsugqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1hsuhn8</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>The favorite!!</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsuhn8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1hsuud0</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I stop this from happening </t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8n3r70zdztae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1hsuwb7</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What shape suits me better </t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsuwb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1hsutu3</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Red gems for my wedding ❤️</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsutu3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1hsuq2g</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dipped today think she did a fast job </t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsuq2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1hsunvh</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>New Years natural nails 🎇🎆</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d896ruj2ytae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1hsujf5</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>new year, new nails 💅🏻😍</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9eckqm4xtae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1hsuaza</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Stiletto or square for my hands?</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsuaza</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1hsua9f</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Gems 💎</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsua9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1hstwp7</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Cheers to 2025🥂</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hstwp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1hstude</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Update dollar tree wraps </t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hstude</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1hstpw0</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>My first attempt on magnetic nail polish, how did I do?</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mue9d3g4rtae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1hsto9u</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>love</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rgyhtebsqtae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1hsspss</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Did my nails for the first time</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3mwuif6tjtae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1hss777</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Christmas Set before removal</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2v3ujlv3gtae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1hss0pv</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Who says you can't get fluorescent yellow in January?</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9h8hrtpetae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1hsrgxq</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>I (unintentionally) did my nails to match my husband’s glasses</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsrgxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1hsrdfs</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Sparkly icy baby french for January ❄️🤍</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8d95yj0atae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1hsr990</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">love my nails without polish </t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6552ao059tae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1hsr7kr</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best press on nail glue avaliable for purchase in europe? </t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hsr7kr/best_press_on_nail_glue_avaliable_for_purchase_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1hsr06c</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>First set of nails for 2025!  My husband said they are so me!  He isn’t wrong! Pink and Blingy and Hello Kitty</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsr06c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1hsqrx8</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New year… new nails </t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsqrx8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1hsqhd1</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>1st set of 2025</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/50qc2aqh3tae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1hsqe0q</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best place to online order cheap, short press-ons? </t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsqe0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1hsqard</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink with white chrome for the new year </t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7oaibl032tae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1hspawk</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Soft pink nails with glitter. ✨️🎀</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hspawk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1hso9ta</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Inspired by graffiti &amp; stickerbomb drift cars</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hso9ta/inspired_by_graffiti_stickerbomb_drift_cars/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1hsnxch</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>too thick/shoddy or am i overreacting?</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsnxch</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1hsiv7m</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>best ombre techniques</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hsiv7m/best_ombre_techniques/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1hspluq</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Have finger nails for the first time in my life and don’t know what to do. HELP</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hspluq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1hsppvw</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Working on Vday designs</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikexrqhlxsae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1hspp02</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>First 2025 set &amp; bday nails ⭐️🦋🖤🫧🤩</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzpr2r9fxsae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1hspnjo</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Switched to longer, pointer(ish) almond but the nude stayed🤭 </t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4fu0mh3xsae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1hspjo7</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One year of doing my own nails </t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hspjo7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1hsp1of</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My current nails I had done for New Year’s Eve/my birthday </t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2y7cixassae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1hsp19e</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Year vibes </t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/73t25ik7ssae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1hsoz4z</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Kicking off 2025 with holo glitter ✨🌈</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uktzuihorsae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1hsom1x</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024 the year I started taking care of my nails again </t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsom1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1hso7d3</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>First time using this color</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/shiwkr5plsae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1hso4aq</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>First set of 2025 💖✨️</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hso4aq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1hsm9i8</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>About to go on vacation, this is the set I’m wearing on the way down🤭</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsm9i8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1ht8qit</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Fifty Shades of Greige (Review and Comparisons) 🦄</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht8qit</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1ht7piu</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First try at gradients as a beginner </t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6py5f1mu0xae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1ht7inm</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>What indie brands have the most misleading swatches?</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ht7inm/what_indie_brands_have_the_most_misleading/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1ht6t0k</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Too early for Valentine's Day polishes? </t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8dbmurgrwae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1ht6754</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Which nail shape?</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht6754</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1ht65to</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First Magnetic - Menchie Cat Eye </t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m2h3jc3vkwae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1ht57oy</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>💅🏻 first mani of the year ✨💕</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht57oy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1ht54yz</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Sacrificed a nail to figure this out… what is it and how do I get rid of it (do I need to)</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zoska5cuawae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1ht4f9c</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First ILNP Polish, love the speckles! </t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bly3q3a94wae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1ht4axp</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>BKL One True Love🩶❤️</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht4axp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1ht3q4h</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Any kbshimmer fans?</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gn0i3fyrxvae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1ht306h</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Picky gel allergy? </t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ht306h/picky_gel_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1ht2yqw</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Long lasting mani</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht2yqw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1ht2u5c</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Winter Magic ❄️</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht2u5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1ht2hmu</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Dreamy lilac skittle ✨</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht2hmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1ht2699</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>High Roller by ILNP is dreamy</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dja51246kvae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1ht2135</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>I Believe I Am Powerful Therefore I Am</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht2135</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1ht1lho</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>SOS</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykdao3ogfvae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1ht12t3</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Dupes or better?</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht12t3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1ht0ovs</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>BKL “Choose Life”</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b5y1d1278vae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1ht0bzj</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>new year's holo in a moment of sunshine :D</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rdpr25q45vae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1hszn0h</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sassy Sauce and Rogue Lacquer combo mani </t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hszn0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1hscbpt</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>First New Years design 🥂</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hscbpt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1hsebpp</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Gel Powder Encapsulation Help</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hsebpp/gel_powder_encapsulation_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1hsz1hp</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>First time wearing both and…</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsz1hp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1hsyurc</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>I like to let my friends guess the polish name. One is real, one my husband makes up.</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1ukn7cptuae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1hsyker</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you put press on nails over hard/builder gel? </t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hsyker/can_you_put_press_on_nails_over_hardbuilder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1hsyed9</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Comparing Cock-A-Doodle Doom and I Still Do</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsyed9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1hsybx2</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Is it reflective?</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1s5s7bnppuae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1hsy932</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Trying to stay moisturized in the winter….</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smft25c5puae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1hsxx2n</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Mooncat Sagebrush</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsxx2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1hsxwi1</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First attempt at baby boomer nails using mica powder </t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xyja0yuhmuae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1hsxtzt</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>There's Snow Bunny Like You</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsxtzt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1hsxlhg</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>My latest Frankenpolish - Off Topic</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsxlhg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1hsx6lh</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Does sheer polish chip more easily?</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hsx6lh/does_sheer_polish_chip_more_easily/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1hswyr8</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t xml:space="preserve">If you could only buy one brand’s multichromes, which would it be? </t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hswyr8/if_you_could_only_buy_one_brands_multichromes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1hsww3z</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Patroness of 😺</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsww3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1hswozx</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Snowstorm incoming…calls for glitter!</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hswozx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1hswb73</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Do you keep a record of your polish collection? I decided to try keeping track of my polishes after a small de-stash. Curious to see what colors I’m really wearing in 2025!</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oe6pllofauae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1hsw6og</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink Velvet nails with regular polish! </t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ao90dzrg9uae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1hsvyxe</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Everything I wore in 2024</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsvyxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1hsvycj</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Does anyone know when the next lynb sale will be?</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hsvycj/does_anyone_know_when_the_next_lynb_sale_will_be/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1hsulda</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>ISO LynB Frosted Light Dupe</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsulda</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1hsuaqn</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Gems 💎</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsuaqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1hsu5sa</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Last Unicorn by Cirque Colors ✨🦄</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uptgbbzbutae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1hsu48d</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Does Seche Vite just not work for KB Shimmer polishes for y'all?</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hsu48d/does_seche_vite_just_not_work_for_kb_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1hsu3tv</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Advice on rubber base/builder gel recommendations for nail polish user</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hsu3tv/advice_on_rubber_basebuilder_gel_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1hstvl1</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>It's Like Keeping Up With The Joneses!</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/reqcx2qbstae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1hstl04</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>My first lacquer show off TuT</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8o94fc4qtae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1hstjtf</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Norpsilocin for my birthday</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lybpz3rvptae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1hst9su</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">No smudge top coat and quick dry? </t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hst9su/no_smudge_top_coat_and_quick_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1hst4ea</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Can you mix together a gel and non-gel, or will it never set/dry?</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hst4ea</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1hssz53</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone else starting off 2025 with this polish? </t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vc6eisipltae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1hssvak</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Magnetic holiday nails ✨</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpz56nlxktae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1hsssbo</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to avoid dark lines on the side of the nail when using a horseshoe magnet? </t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a6qk7hubktae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1hssj1m</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>i get the hype now !</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hssj1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1hssfju</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>A Tale of 2 Hands</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hssfju</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1hss98l</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Came for the purples stayed for the reds</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hss98l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1hsrteq</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>ILNP - Starlight</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsrteq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1hsrq3e</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>BKL’s maidenless</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsrq3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1hsrffd</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Let’s bounce neon crème KBShimmer</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsrffd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1hsrcgy</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I think I’m in love with this color and shape combo </t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsrcgy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1hsqlt1</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Attempt at watercolor nails</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsqlt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1hsqg63</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Favorite blurring / ridge filling base coat with no PVB?</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hsqg63/favorite_blurring_ridge_filling_base_coat_with_no/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1hsq4pl</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Wicked theme &amp; first mooncat</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/viyf08ep0tae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1hspzsg</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Perfect combo?!?</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hspzce</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1hspvqm</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>PPU</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hspvqm/ppu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1hsosbg</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>My Glitter/Metallics Removal Method</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsosbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1hsoqiv</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>damage to nail or gel residue</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tbohfmptpsae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1hsonlc</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>🖤❤️Buffalo Check❤️🖤</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsonlc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1hson9i</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>I love neon tips🥹</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hson9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1hsofok</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Is there a way I can achieve this shade myself?</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rt1gesgnsae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1hsnsrx</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Lisa Frank vibes for NYE 🥳🌈</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsnsrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1hsng09</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Turning Pointe is my new favorite polish</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsng09</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1hsmua5</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Pink makes me feel like a princess 💖</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oba6n2hq9sae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1hslyfb</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>My new year mani💜✨✨</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h8n9lw3h1sae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1hslwii</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>No Gets the Chapelle Inspo</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hslwii</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1hslnwe</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>First mani for 2025</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aulc1t2gyrae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1hsl5fq</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Nail polish to match my dog's eyes?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hsl5fq/nail_polish_to_match_my_dogs_eyes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1hskl02</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>My perfect mnbb shade: OPI Bare My Soul</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hskl02</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1hski86</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which one is better; glitter on thumb and ring finger or just plain? Or should I add glitter to all? </t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hski86</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1ht9lo3</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Fun with glitter</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht9lo3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1ht54tf</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Press ons I made for my friends birthday</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/algo7tczawae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1ht51p8</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Some cute ones I did awhile ago :)</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdgqt4k6awae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1ht50am</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>I need a better nude any recs?</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u80htzot9wae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1ht4zgy</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Some cute duckies</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i21vcmwl9wae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1ht4yg8</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>My late Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zyvtdkvb9wae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1ht2ihb</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set </t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wl88k785nvae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1ht27iu</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Double R Diner</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ht27iu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1ht1ovn</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>these beautiful little ones</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/py0yndf8gvae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1ht0w1s</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>New Year's Eve nails for my mum</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2emevbhs9vae1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1hszvzn</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>late post of my festive Christmas x royal Christmas Stones x Bollywood Jewels Nails</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hszvzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1hszuge</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Black jelly polish!</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hszuge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1hszr34</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>My little nails already after New Year’s ! @eloubeauty</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3z9bg7q0vae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1hsze3a</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>First time trying character nail art ft. Strawberry Shortcake 🍓</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsze3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1hsyv1v</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Glass nail trend without gel</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9ai9ujrtuae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1hsyui9</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Lunar year nails!</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsyui9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1hsxinu</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Practicing line work </t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsxinu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1hsxfl0</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Soft plaid and cat eye</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsxfl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1hsv1v7</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Old porcelain inspired set (hand painted press-ons)</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsv1v7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1hsuolb</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>New Years nails 🎇🎆</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zspv4m48ytae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1hstv1u</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Update dollar tree wraps </t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hstv1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1hssu03</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Nezuko Demon Slayer Nail Art</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pasdg8oktae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1hssbop</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer Nails! </t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ts16w01htae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1hso93y</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Inspired by graffiti &amp; stickerbomb drift cars</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hso93y/inspired_by_graffiti_stickerbomb_drift_cars/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1hsno5q</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>What color polygel should i get ?</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hsno5q/what_color_polygel_should_i_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1hsm0fk</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One of my first portraits on a nail and I’m super proud of it </t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26f6ypwz1sae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1hskgiw</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>First set of 2025!</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pubipd4lrae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1hsjyga</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Funfetti doodle nails for myself 💅⭐️</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsjyga</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1hsjwsx</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>The finished Van Gogh Nails ✨</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsjwsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1hsjdi5</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>first set of 2025!</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsjdi5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1hsiwk4</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Here’s my January set ♥️⚜️</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsiwk4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1hsiviz</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Geode nail art tutorial</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nembb5xu1rae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1hsid6s</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Working on my nuance </t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hsid6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1hshp28</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY gel nails with subtle bling </t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hshp28</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jan  5 08:09:22 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_05.xlsx
+++ b/data/collected_data/2025_01_05.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1320"/>
+  <dimension ref="A1:C1499"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22873,6 +22873,3049 @@
         </is>
       </c>
     </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1hu14n3</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Pink gradient nails 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hu14n3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1hu0d4y</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Was I overcharged?</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o36tdpv8m4be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1hu0bk5</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried press on nails for the first time! Rate them </t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hu0bk5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1htzvdd</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">We Got a Picture with the God of War: Phoenix Indie magnetic polish </t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d1hli33rg4be1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1htztv5</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>If people have fake nails on then how do they clip their fingernails?</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1htztv5/if_people_have_fake_nails_on_then_how_do_they/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1htzoic</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Who else loves blue for new year?</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0j5svwge4be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1htzi1w</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fingers tan from lamp </t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1htzi1w/fingers_tan_from_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1htz96q</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>I changed my girl mindset about her solid colors</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htz96q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1htz5de</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Kraken Nails!</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3wqiexb84be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1htyd09</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in LOVE with my kuromi nails </t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1e085o8wz3be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1htycbf</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>First ever acrylic set</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htycbf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1htybbk</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>NYE nails</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lj6vw73ez3be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1htyazw</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second time ever doing gel x nails 💅 </t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htyazw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1hty2yx</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>First time using polygel and solid builder gel</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hty2yx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1htxvmc</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Haven’t painted my nails in months! Hopefully the first of many 2025 sets ✨</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htxvmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1htvoet</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nail shape would suit me best </t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htvoet</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1htw6ms</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Got a new tech. When I tell y’all I am OBSESSED</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9li8lqje3be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1htxtvz</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>i CANNOT get my olive and june press ons to stay no matter what !</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htxtvz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1htxjpr</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>The inspo was opals! 😊</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wlfv7utqr3be1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1htxn04</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dark blue with neon orange ombre with pink Chrome! </t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htxn04</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1htxjxp</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Made a rainbow smoke nail to swatch the new products I got in today!</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ky7ccbyrr3be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1htx7r3</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Simple but cute 💞</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u0odnpggo3be1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1htx5vu</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htx5vu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1htx5e1</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I can’t get over these; they look black without light directly on them </t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ui9zt51sn3be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1htwvh3</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Why does my top coat do this??</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htwvh3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1htwze8</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>New year sparkle webs, and spider!</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htwze8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1htwu0v</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>I was going for a clean girl look</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htwu0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1htws5b</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Never misses!</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kmla4qe9k3be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1htwoxt</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Can’t go wrong with Funny Bunny</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2nvd1acj3be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1htwnl2</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Galaxy French 🌌</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rgxibdd0j3be1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1htwivx</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails done - be honest </t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wbjloqrh3be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1htwike</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">overfiled at the cuticles, stings a bit especially in warm water should i be worried </t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htwike</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1htwd76</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Avoid Hello beauty nails Russian manicure nyc</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1htwd76/avoid_hello_beauty_nails_russian_manicure_nyc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1htw2xn</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>🤡🤡</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htw2xn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1htvwj8</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>First time doing DIY gel set</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htvwj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1htvrn5</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>OPI Press Ons</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1pmj71mda3be1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1htvesz</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>✨💖✨</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htvesz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1htv8k8</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Engagement nails 🤍🥹 </t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htv8k8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1htv72a</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t xml:space="preserve">miffy nails ... first time doing a red set and i love it </t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9j8odla53be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1htuthg</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Icy blue nails for January </t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16u6to1v13be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1htuqzp</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beginner nails </t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ks91kxa913be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1htui7d</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Going to nail salon for the first time , Nervous AF! Any advice?</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1htui7d/going_to_nail_salon_for_the_first_time_nervous_af/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1htuh82</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Obsessed ❄️</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nv1qrctty2be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1htudxs</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>rose gold chrome for my first nails of the year ✨💅🏼</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htudxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1hts33p</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel mani on top of glued on tips </t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hts33p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1htsay1</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Gel Allergy?</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1htsay1/gel_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1htu15u</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Lifting and breakage - should I change product? Or is my technique in need of work?</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htu15u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1htu0ox</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>How to stop nail from bending downwards</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qql03m2su2be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1htu0ky</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat butts! </t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htu0ky</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1httekw</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is gelipotion a legit brand? I can’t seem to find any reviews on it with the exception of their own YouTube shorts and tik toks. </t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1httekw/is_gelipotion_a_legit_brand_i_cant_seem_to_find/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1httqrl</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying to stay away from nudes this year. </t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1httqrl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1httpb6</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 day old acrylics lifting already? </t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1httpb6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1httiof</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Self taught been doing my own nails for 1 Full year now!</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yj1d388kq2be1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1htt72v</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Gel top coat?</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htt72v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1htt52k</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stick On Nails </t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1htt52k/stick_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1htt29m</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first attempt at ombre(?) on my natural nails! </t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htt29m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1htsowk</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>French chrome for the new year</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56of6mdfj2be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1hto4tr</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>How do I remove my acrylic tips at home?</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efmhqz2si1be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1htrzvt</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vintage Tupperware inspired nails done by Michael at Keystone Claws in Lancaster, PA! </t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htrzvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1htnlwm</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>At home manicure that lasts?</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1htnlwm/at_home_manicure_that_lasts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1htoucj</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Are these nails too thick?</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htoucj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1htr8nk</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>beachy nails done by me🫶</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htr8nk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1htqx0a</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>did these today and so happy how they turned out! ✨</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htqx0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1htqrjs</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Got my first ever gel manicure</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htqrjs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1htqlyh</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Little twist on a French </t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crrigwjj22be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1htqe39</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Can still make the whole place shimmer in 2025</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnjnljyq02be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1htqd0b</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails in 2024 💅 </t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htqd0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1htqb27</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did mushroom nails on myself! </t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dr0z4u102be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1htpze0</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>my nails after the end of the year</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wt6ejy1fx1be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1htpw47</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>New years nails. Ditched the bling for the black polish</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r5crxz4mw1be1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1htpsmy</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying chrome </t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htpsmy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1htpio9</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question about the dip process </t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1htpio9/question_about_the_dip_process/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1htpd85</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Trying out some Glamnetic press ons</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htpd85</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1htpaaq</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Do you like black nails?</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zvnic6mkr1be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1htp3r7</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Got my nails done in honor of my cat who passed recently</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/961jkupdq1be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1htp1kk</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some sparkle for new years </t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6pk8i9wp1be1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1htp0or</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press ons applied with builders gel </t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htp0or</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1htnwr5</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Alternative to acrylics?</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1htnwr5/alternative_to_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1htnvlx</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Moons &amp; Stars </t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htnvlx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1htnta6</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💙 First mani of the new year ✨ Starting the new year with some good vibes, Rogue Laquer Twinkling Vibes </t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htnta6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1htnghu</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>My New Year’s Nails ❤️🎀</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxllvk3fd1be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1htn7lq</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>In love with pink 🩷</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ohbdfpweb1be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1htn39o</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>A little sparkle for the new year ✨</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7e7ri2ka1be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1htn06j</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Recent nails 😍</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htn06j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1htmwnw</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome French tip </t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5ikul0791be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1html2t</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Might be my favorite set yet!</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlz38vco61be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1htmen8</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>I think my nails are “over moisturized “</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1htmen8/i_think_my_nails_are_over_moisturized/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1htmgjq</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Dazzling Night</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yt1istto51be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1htmc8f</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It was a Costco haul. Rip. Heard a loud snap and knew. At least it was the pinky— would have cried if it were my pointer or middle finger </t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1er058dq41be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1htm0h3</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>🍒 Velvet</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abn95cy721be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1htlzcb</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Opal chrome for an icy January look❄️</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htlzcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1htlp9u</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time for my 27th Birthday</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/630dgh3tz0be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1htlond</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are the best/most long lasting drugstore nail polish brands? </t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1htlond/what_are_the_bestmost_long_lasting_drugstore_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1htlmd5</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>How to remove glue from Glamnetics press-on nails</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1htlmd5/how_to_remove_glue_from_glamnetics_presson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1htlcsk</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>It’s time to change my nails, what do you recommend?</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htlcsk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1htlb6o</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Only left did I finish🤣 (still practicing using gel😁)</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htlb6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1htla95</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Will I have a hard time getting gel with these? </t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tjmr40ylw0be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1htl7ob</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Filing press-ons?</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1htl7ob/filing_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1htl00d</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Too blue? </t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htl00d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1htjsc6</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Polygel vs Gel X</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1htjsc6/polygel_vs_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1hu0iyd</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Dupe for Pahlish Sailor Mars?</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1t30t8wn4be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1htzzx3</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Oops.</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ycwnfdtai4be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1htz4tf</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Finally got to see Wicked live</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htz4tf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1htz1bl</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 broken nails to start off the new year 🎉 </t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hiv2wm1374be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1htysw7</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>Nails started to peel from the tip of the nails. 😭Never used to do that😭 HOW do I get the peeling to stop? (have not used fake nails or gel.)</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1htysw7/nails_started_to_peel_from_the_tip_of_the_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1htyk58</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>A little Saturday night gaming</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htyk58</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1htxyd5</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you know what these white areas are on my nails? </t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htxyd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1htxcxv</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>finally trying Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htxcxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1htx2ch</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t xml:space="preserve">VIP is Stun.ning. </t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8i96nz3zm3be1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1htwza9</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Flower Child over black really is electric blue!!</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htwza9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1htww22</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Okay I finally get it. ILNP DEEP SPACE</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sovx456bl3be1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1htwlgx</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Filling acrylic nails with polygel</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1htwlgx/filling_acrylic_nails_with_polygel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1htvken</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Got my first magnetic polish and horseshoe magnet</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htvken</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1htv6cb</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>CF dupe of Essie mod square?</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z27a6z8453be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1htuwvf</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>BlissKiss nail mat appreciation post</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1htuwvf/blisskiss_nail_mat_appreciation_post/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1hturvt</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question regarding undertones </t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hturvt/question_regarding_undertones/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1htuq00</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>First Mani of the Year</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htuq00</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1htu1pa</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Psilocin 🍄</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htu1pa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1htt201</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Cant get a cat eye effect :(</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1htt201/cant_get_a_cat_eye_effect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1htt0a6</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Press on nail and glue recommendations?</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1htt0a6/press_on_nail_and_glue_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1htsxw3</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Whatcha Aurora Borealis using  the ILNP Magnet = 💜💜💜 </t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htsxw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1htsvmb</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anything similar? </t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htsvmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1htsqif</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Attacked for Having Fingers</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htsqif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1htrft3</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>Daughter and I’s “Wicked” nails</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htrft3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1htr2e3</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>Nails breaking … switch to acrylics?</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1htr2e3/nails_breaking_switch_to_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1htqpcq</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>We Got a Picture with the God of War - Phoenix Indie</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wu2n2k4a32be1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1htpyic</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>Day 4/365 and I may have already found my most unbeatable polish of the year (Lurid Lacquer, To Yield More Than One Molecule) 🥀🍒🍷🍇</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htpyic</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1htpyc8</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DND (regular) Lacquer </t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1htpyc8/dnd_regular_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1htpnyr</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>In love 💚🩶</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7fvy1umvu1be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1htpn6l</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Death Valley skittle for those who are curious about 10mg Adderall </t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htpn6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1htpik8</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>This glitter is so pretty 😍</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9401wrmkt1be1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1htp9zr</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce Polish – Secrets &amp; Scandals</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htp9zr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1htp96e</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Recommend me a polish to go with my new ring!</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htp96e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1htp2qr</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>True primary green creme recommendation?</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1htp2qr/true_primary_green_creme_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1htp076</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally got my hands on “It’s Showtime!” by Bees Knees Lacquer </t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htp076</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1htov1q</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>Some fire during a polar vortex</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fwualk8go1be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1htnsel</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>Mooncat Sin Eater</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htnsel</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1htns8z</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>💙 First mani of the new year ✨ Starting the new year with some good vibes, Rogue Laquer Twinkling Vibes</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htns8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1htnmr3</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Finally wore this Nov. 2023 PPU beauty</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htnmr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1htn4e7</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Could there be a better time to put on Frosted Light? ❄️ </t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htn4e7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1htmwfg</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>My 2024 favourites ✨🤭 (with bonus stats)</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htmwfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1htmf22</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Couldn’t choose a color so I did both! I love winter colors </t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htmf22</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1htmdhw</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>ILNP Bluebell and Flower Child</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htmdhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1htmbqp</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>I swatched them all!</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w51a1z6n41be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1htlfd0</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>While trying to take a baby photo for grandma I ended up taking some nail photos instead 😅</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d160521qx0be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1htl5nw</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>One of my favs 💫💅</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htl5nw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1htl522</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>First 2025 Mani! Purple themed skittle</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u0at3iobv0be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1htkvkj</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>BKL'S Baldur's Gate 3 collection PART TWO???</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1htkvkj/bkls_baldurs_gate_3_collection_part_two/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1htkuwb</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>Too Pale For Fairy Dust 😭</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpliilmat0be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1htkqf1</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>I can’t stop staring at my nails 😍</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9ugy3ey8s0be1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1htjwh5</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>Noob question- base coat?</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1htjwh5/noob_question_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1htjjap</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Since joining </t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/skyi3rv0j0be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1htj8cy</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>Anyone know a polish/combo that would match?</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r3nsme6mg0be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1htj86c</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>Does anyone have any insight on Monarch Lacquer?</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1htj86c/does_anyone_have_any_insight_on_monarch_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1htis7k</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Testing out a new year gift 🧲 </t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htis7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1htin8c</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>base coat for strengthening nails? also do u wear gloves in the shower?</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1htin8c/base_coat_for_strengthening_nails_also_do_u_wear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1htijwd</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>🩷💜💙❄️Winter Gradient❄️💙💜🩷</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htijwd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1hti4a8</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>Cuticle flooded with gel from salon?</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hti4a8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1htheeh</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>Four of my favorite magnetics</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htheeh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1htggxg</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>BKL - Never Broker A Deal With A Demon</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6m13qowkuzae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>1htflu0</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>Bee's Knees Lacquer - Cheers To 5 Years</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htflu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr">
+        <is>
+          <t>1htf6xt</t>
+        </is>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>Winter shimmers 🤍🩵🩷</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htf6xt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr">
+        <is>
+          <t>1htezdn</t>
+        </is>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>Aphrodisiac 🌸🎀✨️</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htezdn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr">
+        <is>
+          <t>1htexrm</t>
+        </is>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Arcana </t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htexrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr">
+        <is>
+          <t>1htem81</t>
+        </is>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>First Paint of the Year</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htem81</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr">
+        <is>
+          <t>1htegtw</t>
+        </is>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>Dear diary, today is January 4th. I've already painted my nails twice and bought 3 new polishes... Send help.</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htegtw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr">
+        <is>
+          <t>1hte8cw</t>
+        </is>
+      </c>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>Does anyone remember Liquid Lava?</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hte8cw/does_anyone_remember_liquid_lava/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr">
+        <is>
+          <t>1hte35z</t>
+        </is>
+      </c>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glam Nail Polish </t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hte35z/glam_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr">
+        <is>
+          <t>1htdumt</t>
+        </is>
+      </c>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>My super old bottle of Essie’s Ballet Slippers still worked :)</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lq56m6uu5zae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1490">
+      <c r="A1490" t="inlineStr">
+        <is>
+          <t>1htcfgm</t>
+        </is>
+      </c>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>Finally ordered a bunch of nail polishes, first one is KBShimmer What a Catch 💚</t>
+        </is>
+      </c>
+      <c r="C1490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tbrv4qfooyae1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1491">
+      <c r="A1491" t="inlineStr">
+        <is>
+          <t>1htal6q</t>
+        </is>
+      </c>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>Dam Polish Don't Kiss Your Sis (trust the shimmer) swatch request</t>
+        </is>
+      </c>
+      <c r="C1491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1htal6q/dam_polish_dont_kiss_your_sis_trust_the_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1492">
+      <c r="A1492" t="inlineStr">
+        <is>
+          <t>1htycyw</t>
+        </is>
+      </c>
+      <c r="B1492" t="inlineStr">
+        <is>
+          <t>Stuff I made yesterday 💜✨</t>
+        </is>
+      </c>
+      <c r="C1492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htycyw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1493">
+      <c r="A1493" t="inlineStr">
+        <is>
+          <t>1htujui</t>
+        </is>
+      </c>
+      <c r="B1493" t="inlineStr">
+        <is>
+          <t>Moana inspired custom set</t>
+        </is>
+      </c>
+      <c r="C1493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htujui</t>
+        </is>
+      </c>
+    </row>
+    <row r="1494">
+      <c r="A1494" t="inlineStr">
+        <is>
+          <t>1httbph</t>
+        </is>
+      </c>
+      <c r="B1494" t="inlineStr">
+        <is>
+          <t>sos: how are we doing chrome isolation😭</t>
+        </is>
+      </c>
+      <c r="C1494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1httbph</t>
+        </is>
+      </c>
+    </row>
+    <row r="1495">
+      <c r="A1495" t="inlineStr">
+        <is>
+          <t>1hts2ka</t>
+        </is>
+      </c>
+      <c r="B1495" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Progression </t>
+        </is>
+      </c>
+      <c r="C1495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/os89zytce2be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1496">
+      <c r="A1496" t="inlineStr">
+        <is>
+          <t>1htl059</t>
+        </is>
+      </c>
+      <c r="B1496" t="inlineStr">
+        <is>
+          <t>Forest theme nails</t>
+        </is>
+      </c>
+      <c r="C1496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2dgee1fu0be1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1497">
+      <c r="A1497" t="inlineStr">
+        <is>
+          <t>1hthdvg</t>
+        </is>
+      </c>
+      <c r="B1497" t="inlineStr">
+        <is>
+          <t>First time getting nail art done loop</t>
+        </is>
+      </c>
+      <c r="C1497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hthdvg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1498">
+      <c r="A1498" t="inlineStr">
+        <is>
+          <t>1htcg7b</t>
+        </is>
+      </c>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t xml:space="preserve">maroon tip + gold chrome </t>
+        </is>
+      </c>
+      <c r="C1498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htcg7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1499">
+      <c r="A1499" t="inlineStr">
+        <is>
+          <t>1htb405</t>
+        </is>
+      </c>
+      <c r="B1499" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024 in nail art (there are some plain ones on lazy weeks sorry!) </t>
+        </is>
+      </c>
+      <c r="C1499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1htb405</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>